<commit_message>
Se agrega centro de costos a asignaciones, OC y solicitud de viaticos
</commit_message>
<xml_diff>
--- a/public/file_layouts/OC_model.xlsx
+++ b/public/file_layouts/OC_model.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\cite\public\file_layouts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\services\public\file_layouts\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8E7B3B-8BCE-4A1E-9EAB-89F22D72E027}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="253"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="253" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OC" sheetId="8" r:id="rId1"/>
@@ -19,12 +20,19 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Obligaciones!$A$1:$D$69</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">OC!$A$1:$AV$90</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="179021"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="132">
   <si>
     <t>Cant</t>
   </si>
@@ -471,11 +479,14 @@
   <si>
     <t>Importe</t>
   </si>
+  <si>
+    <t>Centro de costos:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
@@ -775,7 +786,7 @@
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="172">
+  <cellXfs count="173">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -897,7 +908,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -1017,6 +1027,38 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1027,18 +1069,63 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1067,91 +1154,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Millares" xfId="4" builtinId="3"/>
-    <cellStyle name="Millares 2" xfId="5"/>
+    <cellStyle name="Millares 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="2" builtinId="5"/>
-    <cellStyle name="常规_Quotation for Civil Works(按年度含SA1104)" xfId="3"/>
+    <cellStyle name="常规_Quotation for Civil Works(按年度含SA1104)" xfId="3" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1188,7 +1202,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6230" name="3 Imagen"/>
+        <xdr:cNvPr id="6230" name="3 Imagen">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000056180000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1298,6 +1318,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1333,6 +1370,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1508,14 +1562,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:BB91"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W86" sqref="W86"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AX10" sqref="AX10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1652,13 +1706,13 @@
       <c r="AJ2" s="36"/>
       <c r="AK2" s="36"/>
       <c r="AL2" s="36"/>
-      <c r="AM2" s="131"/>
-      <c r="AN2" s="131"/>
-      <c r="AO2" s="131"/>
-      <c r="AP2" s="131"/>
+      <c r="AM2" s="137"/>
+      <c r="AN2" s="137"/>
+      <c r="AO2" s="12"/>
+      <c r="AP2" s="12"/>
       <c r="AQ2" s="12"/>
-      <c r="AR2" s="36"/>
-      <c r="AS2" s="36"/>
+      <c r="AR2" s="12"/>
+      <c r="AS2" s="12"/>
       <c r="AT2" s="36"/>
       <c r="AU2" s="12"/>
       <c r="AV2" s="13"/>
@@ -1707,16 +1761,16 @@
       <c r="AJ3" s="36"/>
       <c r="AK3" s="36"/>
       <c r="AL3" s="36"/>
-      <c r="AM3" s="82"/>
-      <c r="AN3" s="83"/>
-      <c r="AO3" s="83"/>
-      <c r="AP3" s="83"/>
-      <c r="AQ3" s="83"/>
-      <c r="AR3" s="83"/>
-      <c r="AS3" s="83"/>
-      <c r="AT3" s="83"/>
-      <c r="AU3" s="83"/>
-      <c r="AV3" s="84"/>
+      <c r="AM3" s="81"/>
+      <c r="AN3" s="82"/>
+      <c r="AO3" s="82"/>
+      <c r="AP3" s="82"/>
+      <c r="AQ3" s="82"/>
+      <c r="AR3" s="82"/>
+      <c r="AS3" s="82"/>
+      <c r="AT3" s="82"/>
+      <c r="AU3" s="82"/>
+      <c r="AV3" s="83"/>
       <c r="AW3" s="46"/>
     </row>
     <row r="4" spans="1:49" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1740,7 +1794,7 @@
       <c r="R4" s="67"/>
       <c r="S4" s="36"/>
       <c r="T4" s="36"/>
-      <c r="U4" s="97" t="s">
+      <c r="U4" s="96" t="s">
         <v>92</v>
       </c>
       <c r="V4" s="67"/>
@@ -1797,7 +1851,7 @@
       <c r="R5" s="67"/>
       <c r="S5" s="36"/>
       <c r="T5" s="36"/>
-      <c r="U5" s="97" t="s">
+      <c r="U5" s="96" t="s">
         <v>125</v>
       </c>
       <c r="V5" s="67"/>
@@ -1852,7 +1906,7 @@
       <c r="R6" s="67"/>
       <c r="S6" s="36"/>
       <c r="T6" s="36"/>
-      <c r="U6" s="97"/>
+      <c r="U6" s="96"/>
       <c r="V6" s="67"/>
       <c r="W6" s="67"/>
       <c r="X6" s="67"/>
@@ -1872,13 +1926,13 @@
       <c r="AJ6" s="36"/>
       <c r="AK6" s="36"/>
       <c r="AL6" s="36"/>
-      <c r="AM6" s="136"/>
-      <c r="AN6" s="136"/>
-      <c r="AO6" s="136"/>
-      <c r="AP6" s="136"/>
-      <c r="AQ6" s="136"/>
-      <c r="AR6" s="136"/>
-      <c r="AS6" s="136"/>
+      <c r="AM6" s="162"/>
+      <c r="AN6" s="162"/>
+      <c r="AO6" s="162"/>
+      <c r="AP6" s="162"/>
+      <c r="AQ6" s="162"/>
+      <c r="AR6" s="162"/>
+      <c r="AS6" s="162"/>
       <c r="AT6" s="12"/>
       <c r="AU6" s="12"/>
       <c r="AV6" s="13"/>
@@ -1905,7 +1959,7 @@
       <c r="R7" s="67"/>
       <c r="S7" s="36"/>
       <c r="T7" s="36"/>
-      <c r="U7" s="97"/>
+      <c r="U7" s="96"/>
       <c r="V7" s="67"/>
       <c r="W7" s="67"/>
       <c r="X7" s="67"/>
@@ -1969,23 +2023,25 @@
       <c r="AC8" s="40"/>
       <c r="AD8" s="40"/>
       <c r="AE8" s="40"/>
-      <c r="AF8" s="3"/>
+      <c r="AF8" s="35" t="s">
+        <v>131</v>
+      </c>
       <c r="AG8" s="40"/>
       <c r="AH8" s="40"/>
       <c r="AI8" s="40"/>
       <c r="AJ8" s="40"/>
       <c r="AK8" s="40"/>
       <c r="AL8" s="40"/>
-      <c r="AM8" s="71"/>
-      <c r="AN8" s="72"/>
-      <c r="AO8" s="72"/>
-      <c r="AP8" s="72"/>
-      <c r="AQ8" s="72"/>
-      <c r="AR8" s="72"/>
-      <c r="AS8" s="72"/>
-      <c r="AT8" s="72"/>
-      <c r="AU8" s="72"/>
-      <c r="AV8" s="147"/>
+      <c r="AM8" s="172"/>
+      <c r="AN8" s="172"/>
+      <c r="AO8" s="171"/>
+      <c r="AP8" s="171"/>
+      <c r="AQ8" s="171"/>
+      <c r="AR8" s="171"/>
+      <c r="AS8" s="171"/>
+      <c r="AT8" s="71"/>
+      <c r="AU8" s="71"/>
+      <c r="AV8" s="127"/>
       <c r="AW8" s="46"/>
     </row>
     <row r="9" spans="1:49" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2068,23 +2124,23 @@
         <v>109</v>
       </c>
       <c r="X10" s="48"/>
-      <c r="Y10" s="128"/>
-      <c r="Z10" s="128"/>
-      <c r="AA10" s="128"/>
-      <c r="AB10" s="128"/>
-      <c r="AC10" s="128"/>
-      <c r="AD10" s="128"/>
-      <c r="AE10" s="129"/>
-      <c r="AF10" s="87"/>
+      <c r="Y10" s="139"/>
+      <c r="Z10" s="139"/>
+      <c r="AA10" s="139"/>
+      <c r="AB10" s="139"/>
+      <c r="AC10" s="139"/>
+      <c r="AD10" s="139"/>
+      <c r="AE10" s="140"/>
+      <c r="AF10" s="86"/>
       <c r="AG10" s="53" t="s">
         <v>75</v>
       </c>
       <c r="AH10" s="48"/>
-      <c r="AI10" s="167">
+      <c r="AI10" s="143">
         <v>6.96</v>
       </c>
-      <c r="AJ10" s="167"/>
-      <c r="AK10" s="167"/>
+      <c r="AJ10" s="143"/>
+      <c r="AK10" s="143"/>
       <c r="AL10" s="53"/>
       <c r="AM10" s="36"/>
       <c r="AN10" s="36"/>
@@ -2163,12 +2219,12 @@
       <c r="C12" s="47"/>
       <c r="D12" s="47"/>
       <c r="E12" s="47"/>
-      <c r="F12" s="127"/>
-      <c r="G12" s="127"/>
-      <c r="H12" s="127"/>
-      <c r="I12" s="127"/>
-      <c r="J12" s="127"/>
-      <c r="K12" s="127"/>
+      <c r="F12" s="138"/>
+      <c r="G12" s="138"/>
+      <c r="H12" s="138"/>
+      <c r="I12" s="138"/>
+      <c r="J12" s="138"/>
+      <c r="K12" s="138"/>
       <c r="L12" s="47"/>
       <c r="M12" s="18" t="s">
         <v>99</v>
@@ -2186,11 +2242,11 @@
       <c r="V12" s="38"/>
       <c r="W12" s="36"/>
       <c r="X12" s="36"/>
-      <c r="Y12" s="128"/>
-      <c r="Z12" s="128"/>
-      <c r="AA12" s="128"/>
-      <c r="AB12" s="128"/>
-      <c r="AC12" s="128"/>
+      <c r="Y12" s="139"/>
+      <c r="Z12" s="139"/>
+      <c r="AA12" s="139"/>
+      <c r="AB12" s="139"/>
+      <c r="AC12" s="139"/>
       <c r="AD12" s="61"/>
       <c r="AE12" s="60"/>
       <c r="AF12" s="47"/>
@@ -2236,8 +2292,8 @@
         <v>101</v>
       </c>
       <c r="S13" s="48"/>
-      <c r="T13" s="77"/>
-      <c r="U13" s="73"/>
+      <c r="T13" s="76"/>
+      <c r="U13" s="72"/>
       <c r="V13" s="48"/>
       <c r="W13" s="49"/>
       <c r="X13" s="47"/>
@@ -2275,7 +2331,7 @@
       <c r="C14" s="36"/>
       <c r="D14" s="36"/>
       <c r="E14" s="36"/>
-      <c r="F14" s="81"/>
+      <c r="F14" s="80"/>
       <c r="G14" s="36"/>
       <c r="H14" s="36"/>
       <c r="I14" s="36"/>
@@ -2321,176 +2377,176 @@
       <c r="AW14" s="46"/>
     </row>
     <row r="15" spans="1:49" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="88"/>
-      <c r="B15" s="89"/>
-      <c r="C15" s="88"/>
-      <c r="D15" s="90"/>
-      <c r="E15" s="90"/>
-      <c r="F15" s="90"/>
-      <c r="G15" s="90"/>
-      <c r="H15" s="90"/>
-      <c r="I15" s="90"/>
-      <c r="J15" s="90"/>
-      <c r="K15" s="90"/>
-      <c r="L15" s="90"/>
-      <c r="M15" s="90"/>
-      <c r="N15" s="90"/>
-      <c r="O15" s="90"/>
-      <c r="P15" s="90"/>
-      <c r="Q15" s="90"/>
-      <c r="R15" s="90"/>
-      <c r="S15" s="90"/>
-      <c r="T15" s="90"/>
-      <c r="U15" s="90"/>
-      <c r="V15" s="90"/>
-      <c r="W15" s="90"/>
-      <c r="X15" s="90"/>
-      <c r="Y15" s="90"/>
-      <c r="Z15" s="90"/>
-      <c r="AA15" s="90"/>
-      <c r="AB15" s="90"/>
-      <c r="AC15" s="90"/>
-      <c r="AD15" s="90"/>
-      <c r="AE15" s="89"/>
-      <c r="AF15" s="108"/>
-      <c r="AG15" s="100"/>
-      <c r="AH15" s="100"/>
-      <c r="AI15" s="101"/>
-      <c r="AJ15" s="99"/>
-      <c r="AK15" s="100"/>
-      <c r="AL15" s="100"/>
-      <c r="AM15" s="101"/>
-      <c r="AN15" s="108" t="s">
+      <c r="A15" s="87"/>
+      <c r="B15" s="88"/>
+      <c r="C15" s="87"/>
+      <c r="D15" s="89"/>
+      <c r="E15" s="89"/>
+      <c r="F15" s="89"/>
+      <c r="G15" s="89"/>
+      <c r="H15" s="89"/>
+      <c r="I15" s="89"/>
+      <c r="J15" s="89"/>
+      <c r="K15" s="89"/>
+      <c r="L15" s="89"/>
+      <c r="M15" s="89"/>
+      <c r="N15" s="89"/>
+      <c r="O15" s="89"/>
+      <c r="P15" s="89"/>
+      <c r="Q15" s="89"/>
+      <c r="R15" s="89"/>
+      <c r="S15" s="89"/>
+      <c r="T15" s="89"/>
+      <c r="U15" s="89"/>
+      <c r="V15" s="89"/>
+      <c r="W15" s="89"/>
+      <c r="X15" s="89"/>
+      <c r="Y15" s="89"/>
+      <c r="Z15" s="89"/>
+      <c r="AA15" s="89"/>
+      <c r="AB15" s="89"/>
+      <c r="AC15" s="89"/>
+      <c r="AD15" s="89"/>
+      <c r="AE15" s="88"/>
+      <c r="AF15" s="107"/>
+      <c r="AG15" s="99"/>
+      <c r="AH15" s="99"/>
+      <c r="AI15" s="100"/>
+      <c r="AJ15" s="98"/>
+      <c r="AK15" s="99"/>
+      <c r="AL15" s="99"/>
+      <c r="AM15" s="100"/>
+      <c r="AN15" s="107" t="s">
         <v>129</v>
       </c>
-      <c r="AO15" s="110"/>
-      <c r="AP15" s="110"/>
-      <c r="AQ15" s="111"/>
-      <c r="AR15" s="108"/>
-      <c r="AS15" s="110" t="s">
+      <c r="AO15" s="109"/>
+      <c r="AP15" s="109"/>
+      <c r="AQ15" s="110"/>
+      <c r="AR15" s="107"/>
+      <c r="AS15" s="109" t="s">
         <v>130</v>
       </c>
-      <c r="AT15" s="100"/>
-      <c r="AU15" s="100"/>
-      <c r="AV15" s="101"/>
+      <c r="AT15" s="99"/>
+      <c r="AU15" s="99"/>
+      <c r="AV15" s="100"/>
       <c r="AW15" s="46"/>
     </row>
     <row r="16" spans="1:49" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="91" t="s">
+      <c r="A16" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="92"/>
-      <c r="C16" s="91"/>
-      <c r="D16" s="93"/>
-      <c r="E16" s="93"/>
-      <c r="F16" s="93"/>
-      <c r="G16" s="93"/>
-      <c r="H16" s="93"/>
-      <c r="I16" s="93"/>
-      <c r="J16" s="93"/>
-      <c r="K16" s="93"/>
-      <c r="L16" s="93"/>
-      <c r="M16" s="93" t="s">
+      <c r="B16" s="91"/>
+      <c r="C16" s="90"/>
+      <c r="D16" s="92"/>
+      <c r="E16" s="92"/>
+      <c r="F16" s="92"/>
+      <c r="G16" s="92"/>
+      <c r="H16" s="92"/>
+      <c r="I16" s="92"/>
+      <c r="J16" s="92"/>
+      <c r="K16" s="92"/>
+      <c r="L16" s="92"/>
+      <c r="M16" s="92" t="s">
         <v>4</v>
       </c>
-      <c r="N16" s="93"/>
-      <c r="O16" s="93"/>
-      <c r="P16" s="93"/>
-      <c r="Q16" s="93"/>
-      <c r="R16" s="93"/>
-      <c r="S16" s="93"/>
-      <c r="T16" s="93"/>
-      <c r="U16" s="93"/>
-      <c r="V16" s="93"/>
-      <c r="W16" s="93"/>
-      <c r="X16" s="93"/>
-      <c r="Y16" s="93"/>
-      <c r="Z16" s="93"/>
-      <c r="AA16" s="93"/>
-      <c r="AB16" s="93"/>
-      <c r="AC16" s="93"/>
-      <c r="AD16" s="93"/>
-      <c r="AE16" s="92"/>
-      <c r="AF16" s="102"/>
-      <c r="AG16" s="109" t="s">
+      <c r="N16" s="92"/>
+      <c r="O16" s="92"/>
+      <c r="P16" s="92"/>
+      <c r="Q16" s="92"/>
+      <c r="R16" s="92"/>
+      <c r="S16" s="92"/>
+      <c r="T16" s="92"/>
+      <c r="U16" s="92"/>
+      <c r="V16" s="92"/>
+      <c r="W16" s="92"/>
+      <c r="X16" s="92"/>
+      <c r="Y16" s="92"/>
+      <c r="Z16" s="92"/>
+      <c r="AA16" s="92"/>
+      <c r="AB16" s="92"/>
+      <c r="AC16" s="92"/>
+      <c r="AD16" s="92"/>
+      <c r="AE16" s="91"/>
+      <c r="AF16" s="101"/>
+      <c r="AG16" s="108" t="s">
         <v>0</v>
       </c>
-      <c r="AH16" s="103"/>
-      <c r="AI16" s="104"/>
-      <c r="AJ16" s="102"/>
-      <c r="AK16" s="109" t="s">
+      <c r="AH16" s="102"/>
+      <c r="AI16" s="103"/>
+      <c r="AJ16" s="101"/>
+      <c r="AK16" s="108" t="s">
         <v>1</v>
       </c>
-      <c r="AL16" s="103"/>
-      <c r="AM16" s="104"/>
-      <c r="AN16" s="112" t="s">
+      <c r="AL16" s="102"/>
+      <c r="AM16" s="103"/>
+      <c r="AN16" s="111" t="s">
         <v>127</v>
       </c>
-      <c r="AO16" s="109"/>
-      <c r="AP16" s="109"/>
-      <c r="AQ16" s="113"/>
-      <c r="AR16" s="112"/>
-      <c r="AS16" s="109" t="s">
+      <c r="AO16" s="108"/>
+      <c r="AP16" s="108"/>
+      <c r="AQ16" s="112"/>
+      <c r="AR16" s="111"/>
+      <c r="AS16" s="108" t="s">
         <v>118</v>
       </c>
-      <c r="AT16" s="109"/>
-      <c r="AU16" s="109"/>
-      <c r="AV16" s="113"/>
+      <c r="AT16" s="108"/>
+      <c r="AU16" s="108"/>
+      <c r="AV16" s="112"/>
       <c r="AW16" s="46"/>
     </row>
     <row r="17" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="A17" s="94"/>
-      <c r="B17" s="95"/>
-      <c r="C17" s="94"/>
-      <c r="D17" s="96"/>
-      <c r="E17" s="96"/>
-      <c r="F17" s="96"/>
-      <c r="G17" s="96"/>
-      <c r="H17" s="96"/>
-      <c r="I17" s="96"/>
-      <c r="J17" s="96"/>
-      <c r="K17" s="96"/>
-      <c r="L17" s="96"/>
-      <c r="M17" s="96"/>
-      <c r="N17" s="96"/>
-      <c r="O17" s="96"/>
-      <c r="P17" s="96"/>
-      <c r="Q17" s="96"/>
-      <c r="R17" s="96"/>
-      <c r="S17" s="96"/>
-      <c r="T17" s="96"/>
-      <c r="U17" s="96"/>
-      <c r="V17" s="96"/>
-      <c r="W17" s="96"/>
-      <c r="X17" s="96"/>
-      <c r="Y17" s="96"/>
-      <c r="Z17" s="96"/>
-      <c r="AA17" s="96"/>
-      <c r="AB17" s="96"/>
-      <c r="AC17" s="96"/>
-      <c r="AD17" s="96"/>
-      <c r="AE17" s="95"/>
-      <c r="AF17" s="105"/>
-      <c r="AG17" s="106"/>
-      <c r="AH17" s="106"/>
-      <c r="AI17" s="107"/>
-      <c r="AJ17" s="105"/>
-      <c r="AK17" s="106"/>
-      <c r="AL17" s="106"/>
-      <c r="AM17" s="107"/>
-      <c r="AN17" s="114" t="s">
+      <c r="A17" s="93"/>
+      <c r="B17" s="94"/>
+      <c r="C17" s="93"/>
+      <c r="D17" s="95"/>
+      <c r="E17" s="95"/>
+      <c r="F17" s="95"/>
+      <c r="G17" s="95"/>
+      <c r="H17" s="95"/>
+      <c r="I17" s="95"/>
+      <c r="J17" s="95"/>
+      <c r="K17" s="95"/>
+      <c r="L17" s="95"/>
+      <c r="M17" s="95"/>
+      <c r="N17" s="95"/>
+      <c r="O17" s="95"/>
+      <c r="P17" s="95"/>
+      <c r="Q17" s="95"/>
+      <c r="R17" s="95"/>
+      <c r="S17" s="95"/>
+      <c r="T17" s="95"/>
+      <c r="U17" s="95"/>
+      <c r="V17" s="95"/>
+      <c r="W17" s="95"/>
+      <c r="X17" s="95"/>
+      <c r="Y17" s="95"/>
+      <c r="Z17" s="95"/>
+      <c r="AA17" s="95"/>
+      <c r="AB17" s="95"/>
+      <c r="AC17" s="95"/>
+      <c r="AD17" s="95"/>
+      <c r="AE17" s="94"/>
+      <c r="AF17" s="104"/>
+      <c r="AG17" s="105"/>
+      <c r="AH17" s="105"/>
+      <c r="AI17" s="106"/>
+      <c r="AJ17" s="104"/>
+      <c r="AK17" s="105"/>
+      <c r="AL17" s="105"/>
+      <c r="AM17" s="106"/>
+      <c r="AN17" s="113" t="s">
         <v>128</v>
       </c>
-      <c r="AO17" s="115"/>
-      <c r="AP17" s="115"/>
-      <c r="AQ17" s="116"/>
-      <c r="AR17" s="105"/>
-      <c r="AS17" s="115" t="s">
+      <c r="AO17" s="114"/>
+      <c r="AP17" s="114"/>
+      <c r="AQ17" s="115"/>
+      <c r="AR17" s="104"/>
+      <c r="AS17" s="114" t="s">
         <v>128</v>
       </c>
-      <c r="AT17" s="106"/>
-      <c r="AU17" s="106"/>
-      <c r="AV17" s="107"/>
+      <c r="AT17" s="105"/>
+      <c r="AU17" s="105"/>
+      <c r="AV17" s="106"/>
       <c r="AW17" s="46"/>
     </row>
     <row r="18" spans="1:51" x14ac:dyDescent="0.2">
@@ -2525,45 +2581,45 @@
       <c r="AC18" s="36"/>
       <c r="AD18" s="36"/>
       <c r="AE18" s="42"/>
-      <c r="AF18" s="156"/>
-      <c r="AG18" s="157"/>
-      <c r="AH18" s="157"/>
-      <c r="AI18" s="124"/>
-      <c r="AJ18" s="122"/>
-      <c r="AK18" s="123"/>
-      <c r="AL18" s="123"/>
-      <c r="AM18" s="124"/>
-      <c r="AN18" s="156"/>
-      <c r="AO18" s="157"/>
-      <c r="AP18" s="157"/>
-      <c r="AQ18" s="124"/>
-      <c r="AR18" s="155"/>
-      <c r="AS18" s="155"/>
-      <c r="AT18" s="155"/>
-      <c r="AU18" s="156"/>
-      <c r="AV18" s="148"/>
+      <c r="AF18" s="149"/>
+      <c r="AG18" s="150"/>
+      <c r="AH18" s="150"/>
+      <c r="AI18" s="123"/>
+      <c r="AJ18" s="121"/>
+      <c r="AK18" s="122"/>
+      <c r="AL18" s="122"/>
+      <c r="AM18" s="123"/>
+      <c r="AN18" s="149"/>
+      <c r="AO18" s="150"/>
+      <c r="AP18" s="150"/>
+      <c r="AQ18" s="123"/>
+      <c r="AR18" s="148"/>
+      <c r="AS18" s="148"/>
+      <c r="AT18" s="148"/>
+      <c r="AU18" s="149"/>
+      <c r="AV18" s="128"/>
       <c r="AW18" s="46"/>
     </row>
     <row r="19" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A19" s="46"/>
       <c r="B19" s="42"/>
       <c r="C19" s="63"/>
-      <c r="D19" s="75"/>
-      <c r="E19" s="75"/>
-      <c r="F19" s="75"/>
-      <c r="G19" s="75"/>
-      <c r="H19" s="75"/>
-      <c r="I19" s="75"/>
-      <c r="J19" s="75"/>
-      <c r="K19" s="75"/>
-      <c r="L19" s="75"/>
-      <c r="M19" s="75"/>
-      <c r="N19" s="75"/>
-      <c r="O19" s="75"/>
-      <c r="P19" s="75"/>
-      <c r="Q19" s="75"/>
-      <c r="R19" s="75"/>
-      <c r="S19" s="75"/>
+      <c r="D19" s="74"/>
+      <c r="E19" s="74"/>
+      <c r="F19" s="74"/>
+      <c r="G19" s="74"/>
+      <c r="H19" s="74"/>
+      <c r="I19" s="74"/>
+      <c r="J19" s="74"/>
+      <c r="K19" s="74"/>
+      <c r="L19" s="74"/>
+      <c r="M19" s="74"/>
+      <c r="N19" s="74"/>
+      <c r="O19" s="74"/>
+      <c r="P19" s="74"/>
+      <c r="Q19" s="74"/>
+      <c r="R19" s="74"/>
+      <c r="S19" s="74"/>
       <c r="T19" s="36"/>
       <c r="U19" s="36"/>
       <c r="V19" s="36"/>
@@ -2576,30 +2632,30 @@
       <c r="AC19" s="36"/>
       <c r="AD19" s="36"/>
       <c r="AE19" s="42"/>
-      <c r="AF19" s="154"/>
-      <c r="AG19" s="168"/>
-      <c r="AH19" s="168"/>
-      <c r="AI19" s="165"/>
-      <c r="AJ19" s="119"/>
-      <c r="AK19" s="120"/>
-      <c r="AL19" s="120"/>
-      <c r="AM19" s="121"/>
-      <c r="AN19" s="158"/>
-      <c r="AO19" s="159"/>
-      <c r="AP19" s="159"/>
-      <c r="AQ19" s="121"/>
-      <c r="AR19" s="153"/>
-      <c r="AS19" s="153"/>
-      <c r="AT19" s="153"/>
-      <c r="AU19" s="154"/>
-      <c r="AV19" s="149"/>
+      <c r="AF19" s="142"/>
+      <c r="AG19" s="144"/>
+      <c r="AH19" s="144"/>
+      <c r="AI19" s="134"/>
+      <c r="AJ19" s="118"/>
+      <c r="AK19" s="119"/>
+      <c r="AL19" s="119"/>
+      <c r="AM19" s="120"/>
+      <c r="AN19" s="145"/>
+      <c r="AO19" s="146"/>
+      <c r="AP19" s="146"/>
+      <c r="AQ19" s="120"/>
+      <c r="AR19" s="141"/>
+      <c r="AS19" s="141"/>
+      <c r="AT19" s="141"/>
+      <c r="AU19" s="142"/>
+      <c r="AV19" s="129"/>
       <c r="AW19" s="46"/>
     </row>
     <row r="20" spans="1:51" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="66">
         <v>1</v>
       </c>
-      <c r="B20" s="78"/>
+      <c r="B20" s="77"/>
       <c r="C20" s="66"/>
       <c r="D20" s="34"/>
       <c r="E20" s="34"/>
@@ -2628,38 +2684,38 @@
       <c r="AB20" s="34"/>
       <c r="AC20" s="34"/>
       <c r="AD20" s="34"/>
-      <c r="AE20" s="78"/>
-      <c r="AF20" s="154">
+      <c r="AE20" s="77"/>
+      <c r="AF20" s="142">
         <v>1</v>
       </c>
-      <c r="AG20" s="168"/>
-      <c r="AH20" s="168"/>
-      <c r="AI20" s="165"/>
-      <c r="AJ20" s="119" t="s">
+      <c r="AG20" s="144"/>
+      <c r="AH20" s="144"/>
+      <c r="AI20" s="134"/>
+      <c r="AJ20" s="118" t="s">
         <v>119</v>
       </c>
-      <c r="AK20" s="120"/>
-      <c r="AL20" s="120"/>
-      <c r="AM20" s="121"/>
-      <c r="AN20" s="158"/>
-      <c r="AO20" s="159"/>
-      <c r="AP20" s="159"/>
-      <c r="AQ20" s="121"/>
-      <c r="AR20" s="153">
+      <c r="AK20" s="119"/>
+      <c r="AL20" s="119"/>
+      <c r="AM20" s="120"/>
+      <c r="AN20" s="145"/>
+      <c r="AO20" s="146"/>
+      <c r="AP20" s="146"/>
+      <c r="AQ20" s="120"/>
+      <c r="AR20" s="141">
         <f>+AN20*AF20</f>
         <v>0</v>
       </c>
-      <c r="AS20" s="153"/>
-      <c r="AT20" s="153"/>
-      <c r="AU20" s="154"/>
-      <c r="AV20" s="150"/>
-      <c r="AW20" s="79"/>
+      <c r="AS20" s="141"/>
+      <c r="AT20" s="141"/>
+      <c r="AU20" s="142"/>
+      <c r="AV20" s="130"/>
+      <c r="AW20" s="78"/>
       <c r="AX20" s="27"/>
       <c r="AY20" s="27"/>
     </row>
     <row r="21" spans="1:51" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="66"/>
-      <c r="B21" s="78"/>
+      <c r="B21" s="77"/>
       <c r="C21" s="66"/>
       <c r="D21" s="34"/>
       <c r="E21" s="34"/>
@@ -2688,31 +2744,31 @@
       <c r="AB21" s="34"/>
       <c r="AC21" s="34"/>
       <c r="AD21" s="34"/>
-      <c r="AE21" s="78"/>
-      <c r="AF21" s="154"/>
-      <c r="AG21" s="168"/>
-      <c r="AH21" s="168"/>
-      <c r="AI21" s="165"/>
-      <c r="AJ21" s="119"/>
-      <c r="AK21" s="120"/>
-      <c r="AL21" s="120"/>
-      <c r="AM21" s="121"/>
-      <c r="AN21" s="158"/>
-      <c r="AO21" s="159"/>
-      <c r="AP21" s="159"/>
-      <c r="AQ21" s="121"/>
-      <c r="AR21" s="153"/>
-      <c r="AS21" s="153"/>
-      <c r="AT21" s="153"/>
-      <c r="AU21" s="154"/>
-      <c r="AV21" s="149"/>
-      <c r="AW21" s="79"/>
+      <c r="AE21" s="77"/>
+      <c r="AF21" s="142"/>
+      <c r="AG21" s="144"/>
+      <c r="AH21" s="144"/>
+      <c r="AI21" s="134"/>
+      <c r="AJ21" s="118"/>
+      <c r="AK21" s="119"/>
+      <c r="AL21" s="119"/>
+      <c r="AM21" s="120"/>
+      <c r="AN21" s="145"/>
+      <c r="AO21" s="146"/>
+      <c r="AP21" s="146"/>
+      <c r="AQ21" s="120"/>
+      <c r="AR21" s="141"/>
+      <c r="AS21" s="141"/>
+      <c r="AT21" s="141"/>
+      <c r="AU21" s="142"/>
+      <c r="AV21" s="129"/>
+      <c r="AW21" s="78"/>
       <c r="AX21" s="27"/>
       <c r="AY21" s="27"/>
     </row>
     <row r="22" spans="1:51" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="66"/>
-      <c r="B22" s="78"/>
+      <c r="B22" s="77"/>
       <c r="C22" s="66"/>
       <c r="D22" s="34"/>
       <c r="E22" s="34"/>
@@ -2741,31 +2797,31 @@
       <c r="AB22" s="34"/>
       <c r="AC22" s="34"/>
       <c r="AD22" s="34"/>
-      <c r="AE22" s="78"/>
-      <c r="AF22" s="154"/>
-      <c r="AG22" s="168"/>
-      <c r="AH22" s="168"/>
-      <c r="AI22" s="165"/>
-      <c r="AJ22" s="119"/>
-      <c r="AK22" s="120"/>
-      <c r="AL22" s="120"/>
-      <c r="AM22" s="121"/>
-      <c r="AN22" s="158"/>
-      <c r="AO22" s="159"/>
-      <c r="AP22" s="159"/>
-      <c r="AQ22" s="121"/>
-      <c r="AR22" s="153"/>
-      <c r="AS22" s="153"/>
-      <c r="AT22" s="153"/>
-      <c r="AU22" s="154"/>
-      <c r="AV22" s="149"/>
-      <c r="AW22" s="79"/>
+      <c r="AE22" s="77"/>
+      <c r="AF22" s="142"/>
+      <c r="AG22" s="144"/>
+      <c r="AH22" s="144"/>
+      <c r="AI22" s="134"/>
+      <c r="AJ22" s="118"/>
+      <c r="AK22" s="119"/>
+      <c r="AL22" s="119"/>
+      <c r="AM22" s="120"/>
+      <c r="AN22" s="145"/>
+      <c r="AO22" s="146"/>
+      <c r="AP22" s="146"/>
+      <c r="AQ22" s="120"/>
+      <c r="AR22" s="141"/>
+      <c r="AS22" s="141"/>
+      <c r="AT22" s="141"/>
+      <c r="AU22" s="142"/>
+      <c r="AV22" s="129"/>
+      <c r="AW22" s="78"/>
       <c r="AX22" s="27"/>
       <c r="AY22" s="27"/>
     </row>
     <row r="23" spans="1:51" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="66"/>
-      <c r="B23" s="78"/>
+      <c r="B23" s="77"/>
       <c r="C23" s="66"/>
       <c r="D23" s="34"/>
       <c r="E23" s="34"/>
@@ -2794,29 +2850,29 @@
       <c r="AB23" s="34"/>
       <c r="AC23" s="34"/>
       <c r="AD23" s="34"/>
-      <c r="AE23" s="78"/>
-      <c r="AF23" s="154"/>
-      <c r="AG23" s="168"/>
-      <c r="AH23" s="168"/>
-      <c r="AI23" s="165"/>
-      <c r="AJ23" s="119"/>
-      <c r="AK23" s="120"/>
-      <c r="AL23" s="120"/>
-      <c r="AM23" s="121"/>
-      <c r="AN23" s="158"/>
-      <c r="AO23" s="159"/>
-      <c r="AP23" s="159"/>
-      <c r="AQ23" s="121"/>
-      <c r="AR23" s="153"/>
-      <c r="AS23" s="153"/>
-      <c r="AT23" s="153"/>
-      <c r="AU23" s="154"/>
-      <c r="AV23" s="149"/>
+      <c r="AE23" s="77"/>
+      <c r="AF23" s="142"/>
+      <c r="AG23" s="144"/>
+      <c r="AH23" s="144"/>
+      <c r="AI23" s="134"/>
+      <c r="AJ23" s="118"/>
+      <c r="AK23" s="119"/>
+      <c r="AL23" s="119"/>
+      <c r="AM23" s="120"/>
+      <c r="AN23" s="145"/>
+      <c r="AO23" s="146"/>
+      <c r="AP23" s="146"/>
+      <c r="AQ23" s="120"/>
+      <c r="AR23" s="141"/>
+      <c r="AS23" s="141"/>
+      <c r="AT23" s="141"/>
+      <c r="AU23" s="142"/>
+      <c r="AV23" s="129"/>
       <c r="AW23" s="66"/>
     </row>
     <row r="24" spans="1:51" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="66"/>
-      <c r="B24" s="78"/>
+      <c r="B24" s="77"/>
       <c r="C24" s="66"/>
       <c r="D24" s="34"/>
       <c r="E24" s="34"/>
@@ -2845,29 +2901,29 @@
       <c r="AB24" s="34"/>
       <c r="AC24" s="34"/>
       <c r="AD24" s="34"/>
-      <c r="AE24" s="78"/>
-      <c r="AF24" s="154"/>
-      <c r="AG24" s="168"/>
-      <c r="AH24" s="168"/>
-      <c r="AI24" s="165"/>
-      <c r="AJ24" s="119"/>
-      <c r="AK24" s="120"/>
-      <c r="AL24" s="120"/>
-      <c r="AM24" s="121"/>
-      <c r="AN24" s="158"/>
-      <c r="AO24" s="159"/>
-      <c r="AP24" s="159"/>
-      <c r="AQ24" s="121"/>
-      <c r="AR24" s="153"/>
-      <c r="AS24" s="153"/>
-      <c r="AT24" s="153"/>
-      <c r="AU24" s="154"/>
-      <c r="AV24" s="149"/>
+      <c r="AE24" s="77"/>
+      <c r="AF24" s="142"/>
+      <c r="AG24" s="144"/>
+      <c r="AH24" s="144"/>
+      <c r="AI24" s="134"/>
+      <c r="AJ24" s="118"/>
+      <c r="AK24" s="119"/>
+      <c r="AL24" s="119"/>
+      <c r="AM24" s="120"/>
+      <c r="AN24" s="145"/>
+      <c r="AO24" s="146"/>
+      <c r="AP24" s="146"/>
+      <c r="AQ24" s="120"/>
+      <c r="AR24" s="141"/>
+      <c r="AS24" s="141"/>
+      <c r="AT24" s="141"/>
+      <c r="AU24" s="142"/>
+      <c r="AV24" s="129"/>
       <c r="AW24" s="66"/>
     </row>
     <row r="25" spans="1:51" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="66"/>
-      <c r="B25" s="78"/>
+      <c r="B25" s="77"/>
       <c r="C25" s="66"/>
       <c r="D25" s="34"/>
       <c r="E25" s="34"/>
@@ -2896,30 +2952,30 @@
       <c r="AB25" s="34"/>
       <c r="AC25" s="34"/>
       <c r="AD25" s="34"/>
-      <c r="AE25" s="78"/>
-      <c r="AF25" s="154"/>
-      <c r="AG25" s="168"/>
-      <c r="AH25" s="168"/>
-      <c r="AI25" s="165"/>
-      <c r="AJ25" s="119"/>
-      <c r="AK25" s="120"/>
-      <c r="AL25" s="120"/>
-      <c r="AM25" s="121"/>
-      <c r="AN25" s="158"/>
-      <c r="AO25" s="159"/>
-      <c r="AP25" s="159"/>
-      <c r="AQ25" s="121"/>
-      <c r="AR25" s="153"/>
-      <c r="AS25" s="153"/>
-      <c r="AT25" s="153"/>
-      <c r="AU25" s="154"/>
-      <c r="AV25" s="149"/>
-      <c r="AW25" s="79"/>
+      <c r="AE25" s="77"/>
+      <c r="AF25" s="142"/>
+      <c r="AG25" s="144"/>
+      <c r="AH25" s="144"/>
+      <c r="AI25" s="134"/>
+      <c r="AJ25" s="118"/>
+      <c r="AK25" s="119"/>
+      <c r="AL25" s="119"/>
+      <c r="AM25" s="120"/>
+      <c r="AN25" s="145"/>
+      <c r="AO25" s="146"/>
+      <c r="AP25" s="146"/>
+      <c r="AQ25" s="120"/>
+      <c r="AR25" s="141"/>
+      <c r="AS25" s="141"/>
+      <c r="AT25" s="141"/>
+      <c r="AU25" s="142"/>
+      <c r="AV25" s="129"/>
+      <c r="AW25" s="78"/>
       <c r="AY25" s="29"/>
     </row>
     <row r="26" spans="1:51" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="66"/>
-      <c r="B26" s="78"/>
+      <c r="B26" s="77"/>
       <c r="C26" s="66"/>
       <c r="D26" s="34"/>
       <c r="E26" s="34"/>
@@ -2948,30 +3004,30 @@
       <c r="AB26" s="34"/>
       <c r="AC26" s="34"/>
       <c r="AD26" s="34"/>
-      <c r="AE26" s="78"/>
-      <c r="AF26" s="154"/>
-      <c r="AG26" s="168"/>
-      <c r="AH26" s="168"/>
-      <c r="AI26" s="165"/>
-      <c r="AJ26" s="119"/>
-      <c r="AK26" s="120"/>
-      <c r="AL26" s="120"/>
-      <c r="AM26" s="121"/>
-      <c r="AN26" s="158"/>
-      <c r="AO26" s="159"/>
-      <c r="AP26" s="159"/>
-      <c r="AQ26" s="121"/>
-      <c r="AR26" s="153"/>
-      <c r="AS26" s="153"/>
-      <c r="AT26" s="153"/>
-      <c r="AU26" s="154"/>
-      <c r="AV26" s="149"/>
-      <c r="AW26" s="79"/>
+      <c r="AE26" s="77"/>
+      <c r="AF26" s="142"/>
+      <c r="AG26" s="144"/>
+      <c r="AH26" s="144"/>
+      <c r="AI26" s="134"/>
+      <c r="AJ26" s="118"/>
+      <c r="AK26" s="119"/>
+      <c r="AL26" s="119"/>
+      <c r="AM26" s="120"/>
+      <c r="AN26" s="145"/>
+      <c r="AO26" s="146"/>
+      <c r="AP26" s="146"/>
+      <c r="AQ26" s="120"/>
+      <c r="AR26" s="141"/>
+      <c r="AS26" s="141"/>
+      <c r="AT26" s="141"/>
+      <c r="AU26" s="142"/>
+      <c r="AV26" s="129"/>
+      <c r="AW26" s="78"/>
       <c r="AY26" s="29"/>
     </row>
     <row r="27" spans="1:51" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="66"/>
-      <c r="B27" s="78"/>
+      <c r="B27" s="77"/>
       <c r="C27" s="66"/>
       <c r="D27" s="34"/>
       <c r="E27" s="34"/>
@@ -3000,29 +3056,29 @@
       <c r="AB27" s="34"/>
       <c r="AC27" s="34"/>
       <c r="AD27" s="34"/>
-      <c r="AE27" s="78"/>
-      <c r="AF27" s="154"/>
-      <c r="AG27" s="168"/>
-      <c r="AH27" s="168"/>
-      <c r="AI27" s="165"/>
-      <c r="AJ27" s="119"/>
-      <c r="AK27" s="120"/>
-      <c r="AL27" s="120"/>
-      <c r="AM27" s="121"/>
-      <c r="AN27" s="158"/>
-      <c r="AO27" s="159"/>
-      <c r="AP27" s="159"/>
-      <c r="AQ27" s="121"/>
-      <c r="AR27" s="153"/>
-      <c r="AS27" s="153"/>
-      <c r="AT27" s="153"/>
-      <c r="AU27" s="154"/>
-      <c r="AV27" s="149"/>
-      <c r="AW27" s="79"/>
+      <c r="AE27" s="77"/>
+      <c r="AF27" s="142"/>
+      <c r="AG27" s="144"/>
+      <c r="AH27" s="144"/>
+      <c r="AI27" s="134"/>
+      <c r="AJ27" s="118"/>
+      <c r="AK27" s="119"/>
+      <c r="AL27" s="119"/>
+      <c r="AM27" s="120"/>
+      <c r="AN27" s="145"/>
+      <c r="AO27" s="146"/>
+      <c r="AP27" s="146"/>
+      <c r="AQ27" s="120"/>
+      <c r="AR27" s="141"/>
+      <c r="AS27" s="141"/>
+      <c r="AT27" s="141"/>
+      <c r="AU27" s="142"/>
+      <c r="AV27" s="129"/>
+      <c r="AW27" s="78"/>
     </row>
     <row r="28" spans="1:51" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="66"/>
-      <c r="B28" s="78"/>
+      <c r="B28" s="77"/>
       <c r="C28" s="66"/>
       <c r="D28" s="34"/>
       <c r="E28" s="34"/>
@@ -3051,29 +3107,29 @@
       <c r="AB28" s="34"/>
       <c r="AC28" s="34"/>
       <c r="AD28" s="34"/>
-      <c r="AE28" s="78"/>
-      <c r="AF28" s="154"/>
-      <c r="AG28" s="168"/>
-      <c r="AH28" s="168"/>
-      <c r="AI28" s="165"/>
-      <c r="AJ28" s="119"/>
-      <c r="AK28" s="120"/>
-      <c r="AL28" s="120"/>
-      <c r="AM28" s="121"/>
-      <c r="AN28" s="158"/>
-      <c r="AO28" s="159"/>
-      <c r="AP28" s="159"/>
-      <c r="AQ28" s="121"/>
-      <c r="AR28" s="153"/>
-      <c r="AS28" s="153"/>
-      <c r="AT28" s="153"/>
-      <c r="AU28" s="154"/>
-      <c r="AV28" s="149"/>
+      <c r="AE28" s="77"/>
+      <c r="AF28" s="142"/>
+      <c r="AG28" s="144"/>
+      <c r="AH28" s="144"/>
+      <c r="AI28" s="134"/>
+      <c r="AJ28" s="118"/>
+      <c r="AK28" s="119"/>
+      <c r="AL28" s="119"/>
+      <c r="AM28" s="120"/>
+      <c r="AN28" s="145"/>
+      <c r="AO28" s="146"/>
+      <c r="AP28" s="146"/>
+      <c r="AQ28" s="120"/>
+      <c r="AR28" s="141"/>
+      <c r="AS28" s="141"/>
+      <c r="AT28" s="141"/>
+      <c r="AU28" s="142"/>
+      <c r="AV28" s="129"/>
       <c r="AW28" s="66"/>
     </row>
     <row r="29" spans="1:51" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="66"/>
-      <c r="B29" s="78"/>
+      <c r="B29" s="77"/>
       <c r="C29" s="66"/>
       <c r="D29" s="34"/>
       <c r="E29" s="34"/>
@@ -3102,31 +3158,31 @@
       <c r="AB29" s="34"/>
       <c r="AC29" s="34"/>
       <c r="AD29" s="34"/>
-      <c r="AE29" s="78"/>
-      <c r="AF29" s="154"/>
-      <c r="AG29" s="168"/>
-      <c r="AH29" s="168"/>
-      <c r="AI29" s="165"/>
-      <c r="AJ29" s="119"/>
-      <c r="AK29" s="120"/>
-      <c r="AL29" s="120"/>
-      <c r="AM29" s="121"/>
-      <c r="AN29" s="158"/>
-      <c r="AO29" s="159"/>
-      <c r="AP29" s="159"/>
-      <c r="AQ29" s="121"/>
-      <c r="AR29" s="153"/>
-      <c r="AS29" s="153"/>
-      <c r="AT29" s="153"/>
-      <c r="AU29" s="154"/>
-      <c r="AV29" s="149"/>
-      <c r="AW29" s="79"/>
+      <c r="AE29" s="77"/>
+      <c r="AF29" s="142"/>
+      <c r="AG29" s="144"/>
+      <c r="AH29" s="144"/>
+      <c r="AI29" s="134"/>
+      <c r="AJ29" s="118"/>
+      <c r="AK29" s="119"/>
+      <c r="AL29" s="119"/>
+      <c r="AM29" s="120"/>
+      <c r="AN29" s="145"/>
+      <c r="AO29" s="146"/>
+      <c r="AP29" s="146"/>
+      <c r="AQ29" s="120"/>
+      <c r="AR29" s="141"/>
+      <c r="AS29" s="141"/>
+      <c r="AT29" s="141"/>
+      <c r="AU29" s="142"/>
+      <c r="AV29" s="129"/>
+      <c r="AW29" s="78"/>
       <c r="AX29" s="27"/>
       <c r="AY29" s="27"/>
     </row>
     <row r="30" spans="1:51" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="66"/>
-      <c r="B30" s="78"/>
+      <c r="B30" s="77"/>
       <c r="C30" s="66"/>
       <c r="D30" s="34"/>
       <c r="E30" s="34"/>
@@ -3155,31 +3211,31 @@
       <c r="AB30" s="34"/>
       <c r="AC30" s="34"/>
       <c r="AD30" s="34"/>
-      <c r="AE30" s="78"/>
-      <c r="AF30" s="154"/>
-      <c r="AG30" s="168"/>
-      <c r="AH30" s="168"/>
-      <c r="AI30" s="165"/>
-      <c r="AJ30" s="119"/>
-      <c r="AK30" s="120"/>
-      <c r="AL30" s="120"/>
-      <c r="AM30" s="121"/>
-      <c r="AN30" s="158"/>
-      <c r="AO30" s="159"/>
-      <c r="AP30" s="159"/>
-      <c r="AQ30" s="121"/>
-      <c r="AR30" s="153"/>
-      <c r="AS30" s="153"/>
-      <c r="AT30" s="153"/>
-      <c r="AU30" s="154"/>
-      <c r="AV30" s="149"/>
-      <c r="AW30" s="79"/>
+      <c r="AE30" s="77"/>
+      <c r="AF30" s="142"/>
+      <c r="AG30" s="144"/>
+      <c r="AH30" s="144"/>
+      <c r="AI30" s="134"/>
+      <c r="AJ30" s="118"/>
+      <c r="AK30" s="119"/>
+      <c r="AL30" s="119"/>
+      <c r="AM30" s="120"/>
+      <c r="AN30" s="145"/>
+      <c r="AO30" s="146"/>
+      <c r="AP30" s="146"/>
+      <c r="AQ30" s="120"/>
+      <c r="AR30" s="141"/>
+      <c r="AS30" s="141"/>
+      <c r="AT30" s="141"/>
+      <c r="AU30" s="142"/>
+      <c r="AV30" s="129"/>
+      <c r="AW30" s="78"/>
       <c r="AX30" s="27"/>
       <c r="AY30" s="27"/>
     </row>
     <row r="31" spans="1:51" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="66"/>
-      <c r="B31" s="78"/>
+      <c r="B31" s="77"/>
       <c r="C31" s="66"/>
       <c r="D31" s="34"/>
       <c r="E31" s="34"/>
@@ -3208,31 +3264,31 @@
       <c r="AB31" s="34"/>
       <c r="AC31" s="34"/>
       <c r="AD31" s="34"/>
-      <c r="AE31" s="78"/>
-      <c r="AF31" s="154"/>
-      <c r="AG31" s="168"/>
-      <c r="AH31" s="168"/>
-      <c r="AI31" s="165"/>
-      <c r="AJ31" s="119"/>
-      <c r="AK31" s="120"/>
-      <c r="AL31" s="120"/>
-      <c r="AM31" s="121"/>
-      <c r="AN31" s="158"/>
-      <c r="AO31" s="159"/>
-      <c r="AP31" s="159"/>
-      <c r="AQ31" s="121"/>
-      <c r="AR31" s="153"/>
-      <c r="AS31" s="153"/>
-      <c r="AT31" s="153"/>
-      <c r="AU31" s="154"/>
-      <c r="AV31" s="149"/>
-      <c r="AW31" s="79"/>
+      <c r="AE31" s="77"/>
+      <c r="AF31" s="142"/>
+      <c r="AG31" s="144"/>
+      <c r="AH31" s="144"/>
+      <c r="AI31" s="134"/>
+      <c r="AJ31" s="118"/>
+      <c r="AK31" s="119"/>
+      <c r="AL31" s="119"/>
+      <c r="AM31" s="120"/>
+      <c r="AN31" s="145"/>
+      <c r="AO31" s="146"/>
+      <c r="AP31" s="146"/>
+      <c r="AQ31" s="120"/>
+      <c r="AR31" s="141"/>
+      <c r="AS31" s="141"/>
+      <c r="AT31" s="141"/>
+      <c r="AU31" s="142"/>
+      <c r="AV31" s="129"/>
+      <c r="AW31" s="78"/>
       <c r="AX31" s="27"/>
       <c r="AY31" s="27"/>
     </row>
     <row r="32" spans="1:51" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="66"/>
-      <c r="B32" s="78"/>
+      <c r="B32" s="77"/>
       <c r="C32" s="66"/>
       <c r="D32" s="34"/>
       <c r="E32" s="34"/>
@@ -3261,29 +3317,29 @@
       <c r="AB32" s="34"/>
       <c r="AC32" s="34"/>
       <c r="AD32" s="34"/>
-      <c r="AE32" s="78"/>
-      <c r="AF32" s="154"/>
-      <c r="AG32" s="168"/>
-      <c r="AH32" s="168"/>
-      <c r="AI32" s="165"/>
-      <c r="AJ32" s="119"/>
-      <c r="AK32" s="120"/>
-      <c r="AL32" s="120"/>
-      <c r="AM32" s="121"/>
-      <c r="AN32" s="158"/>
-      <c r="AO32" s="159"/>
-      <c r="AP32" s="159"/>
-      <c r="AQ32" s="121"/>
-      <c r="AR32" s="153"/>
-      <c r="AS32" s="153"/>
-      <c r="AT32" s="153"/>
-      <c r="AU32" s="154"/>
-      <c r="AV32" s="149"/>
+      <c r="AE32" s="77"/>
+      <c r="AF32" s="142"/>
+      <c r="AG32" s="144"/>
+      <c r="AH32" s="144"/>
+      <c r="AI32" s="134"/>
+      <c r="AJ32" s="118"/>
+      <c r="AK32" s="119"/>
+      <c r="AL32" s="119"/>
+      <c r="AM32" s="120"/>
+      <c r="AN32" s="145"/>
+      <c r="AO32" s="146"/>
+      <c r="AP32" s="146"/>
+      <c r="AQ32" s="120"/>
+      <c r="AR32" s="141"/>
+      <c r="AS32" s="141"/>
+      <c r="AT32" s="141"/>
+      <c r="AU32" s="142"/>
+      <c r="AV32" s="129"/>
       <c r="AW32" s="66"/>
     </row>
     <row r="33" spans="1:49" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="66"/>
-      <c r="B33" s="78"/>
+      <c r="B33" s="77"/>
       <c r="C33" s="66"/>
       <c r="D33" s="34"/>
       <c r="E33" s="34"/>
@@ -3312,29 +3368,29 @@
       <c r="AB33" s="34"/>
       <c r="AC33" s="34"/>
       <c r="AD33" s="34"/>
-      <c r="AE33" s="78"/>
-      <c r="AF33" s="154"/>
-      <c r="AG33" s="168"/>
-      <c r="AH33" s="168"/>
-      <c r="AI33" s="165"/>
-      <c r="AJ33" s="119"/>
-      <c r="AK33" s="120"/>
-      <c r="AL33" s="120"/>
-      <c r="AM33" s="121"/>
-      <c r="AN33" s="158"/>
-      <c r="AO33" s="159"/>
-      <c r="AP33" s="159"/>
-      <c r="AQ33" s="121"/>
-      <c r="AR33" s="153"/>
-      <c r="AS33" s="153"/>
-      <c r="AT33" s="153"/>
-      <c r="AU33" s="154"/>
-      <c r="AV33" s="149"/>
+      <c r="AE33" s="77"/>
+      <c r="AF33" s="142"/>
+      <c r="AG33" s="144"/>
+      <c r="AH33" s="144"/>
+      <c r="AI33" s="134"/>
+      <c r="AJ33" s="118"/>
+      <c r="AK33" s="119"/>
+      <c r="AL33" s="119"/>
+      <c r="AM33" s="120"/>
+      <c r="AN33" s="145"/>
+      <c r="AO33" s="146"/>
+      <c r="AP33" s="146"/>
+      <c r="AQ33" s="120"/>
+      <c r="AR33" s="141"/>
+      <c r="AS33" s="141"/>
+      <c r="AT33" s="141"/>
+      <c r="AU33" s="142"/>
+      <c r="AV33" s="129"/>
       <c r="AW33" s="66"/>
     </row>
     <row r="34" spans="1:49" s="28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="66"/>
-      <c r="B34" s="78"/>
+      <c r="B34" s="77"/>
       <c r="C34" s="66"/>
       <c r="D34" s="34"/>
       <c r="E34" s="34"/>
@@ -3363,24 +3419,24 @@
       <c r="AB34" s="34"/>
       <c r="AC34" s="34"/>
       <c r="AD34" s="34"/>
-      <c r="AE34" s="78"/>
-      <c r="AF34" s="154"/>
-      <c r="AG34" s="168"/>
-      <c r="AH34" s="168"/>
-      <c r="AI34" s="165"/>
-      <c r="AJ34" s="119"/>
-      <c r="AK34" s="120"/>
-      <c r="AL34" s="120"/>
-      <c r="AM34" s="121"/>
-      <c r="AN34" s="158"/>
-      <c r="AO34" s="159"/>
-      <c r="AP34" s="159"/>
-      <c r="AQ34" s="121"/>
-      <c r="AR34" s="153"/>
-      <c r="AS34" s="153"/>
-      <c r="AT34" s="153"/>
-      <c r="AU34" s="154"/>
-      <c r="AV34" s="149"/>
+      <c r="AE34" s="77"/>
+      <c r="AF34" s="142"/>
+      <c r="AG34" s="144"/>
+      <c r="AH34" s="144"/>
+      <c r="AI34" s="134"/>
+      <c r="AJ34" s="118"/>
+      <c r="AK34" s="119"/>
+      <c r="AL34" s="119"/>
+      <c r="AM34" s="120"/>
+      <c r="AN34" s="145"/>
+      <c r="AO34" s="146"/>
+      <c r="AP34" s="146"/>
+      <c r="AQ34" s="120"/>
+      <c r="AR34" s="141"/>
+      <c r="AS34" s="141"/>
+      <c r="AT34" s="141"/>
+      <c r="AU34" s="142"/>
+      <c r="AV34" s="129"/>
       <c r="AW34" s="66"/>
     </row>
     <row r="35" spans="1:49" x14ac:dyDescent="0.2">
@@ -3415,23 +3471,23 @@
       <c r="AC35" s="36"/>
       <c r="AD35" s="36"/>
       <c r="AE35" s="42"/>
-      <c r="AF35" s="154"/>
-      <c r="AG35" s="168"/>
-      <c r="AH35" s="168"/>
-      <c r="AI35" s="165"/>
-      <c r="AJ35" s="119"/>
-      <c r="AK35" s="120"/>
-      <c r="AL35" s="120"/>
-      <c r="AM35" s="121"/>
-      <c r="AN35" s="158"/>
-      <c r="AO35" s="159"/>
-      <c r="AP35" s="159"/>
-      <c r="AQ35" s="121"/>
-      <c r="AR35" s="153"/>
-      <c r="AS35" s="153"/>
-      <c r="AT35" s="153"/>
-      <c r="AU35" s="154"/>
-      <c r="AV35" s="149"/>
+      <c r="AF35" s="142"/>
+      <c r="AG35" s="144"/>
+      <c r="AH35" s="144"/>
+      <c r="AI35" s="134"/>
+      <c r="AJ35" s="118"/>
+      <c r="AK35" s="119"/>
+      <c r="AL35" s="119"/>
+      <c r="AM35" s="120"/>
+      <c r="AN35" s="145"/>
+      <c r="AO35" s="146"/>
+      <c r="AP35" s="146"/>
+      <c r="AQ35" s="120"/>
+      <c r="AR35" s="141"/>
+      <c r="AS35" s="141"/>
+      <c r="AT35" s="141"/>
+      <c r="AU35" s="142"/>
+      <c r="AV35" s="129"/>
       <c r="AW35" s="46"/>
     </row>
     <row r="36" spans="1:49" x14ac:dyDescent="0.2">
@@ -3466,23 +3522,23 @@
       <c r="AC36" s="36"/>
       <c r="AD36" s="36"/>
       <c r="AE36" s="42"/>
-      <c r="AF36" s="154"/>
-      <c r="AG36" s="168"/>
-      <c r="AH36" s="168"/>
-      <c r="AI36" s="165"/>
-      <c r="AJ36" s="119"/>
-      <c r="AK36" s="120"/>
-      <c r="AL36" s="120"/>
-      <c r="AM36" s="121"/>
-      <c r="AN36" s="158"/>
-      <c r="AO36" s="159"/>
-      <c r="AP36" s="159"/>
-      <c r="AQ36" s="121"/>
-      <c r="AR36" s="153"/>
-      <c r="AS36" s="153"/>
-      <c r="AT36" s="153"/>
-      <c r="AU36" s="154"/>
-      <c r="AV36" s="149"/>
+      <c r="AF36" s="142"/>
+      <c r="AG36" s="144"/>
+      <c r="AH36" s="144"/>
+      <c r="AI36" s="134"/>
+      <c r="AJ36" s="118"/>
+      <c r="AK36" s="119"/>
+      <c r="AL36" s="119"/>
+      <c r="AM36" s="120"/>
+      <c r="AN36" s="145"/>
+      <c r="AO36" s="146"/>
+      <c r="AP36" s="146"/>
+      <c r="AQ36" s="120"/>
+      <c r="AR36" s="141"/>
+      <c r="AS36" s="141"/>
+      <c r="AT36" s="141"/>
+      <c r="AU36" s="142"/>
+      <c r="AV36" s="129"/>
       <c r="AW36" s="46"/>
     </row>
     <row r="37" spans="1:49" x14ac:dyDescent="0.2">
@@ -3517,23 +3573,23 @@
       <c r="AC37" s="36"/>
       <c r="AD37" s="36"/>
       <c r="AE37" s="42"/>
-      <c r="AF37" s="154"/>
-      <c r="AG37" s="168"/>
-      <c r="AH37" s="168"/>
-      <c r="AI37" s="165"/>
-      <c r="AJ37" s="119"/>
-      <c r="AK37" s="120"/>
-      <c r="AL37" s="120"/>
-      <c r="AM37" s="121"/>
-      <c r="AN37" s="158"/>
-      <c r="AO37" s="159"/>
-      <c r="AP37" s="159"/>
-      <c r="AQ37" s="121"/>
-      <c r="AR37" s="153"/>
-      <c r="AS37" s="153"/>
-      <c r="AT37" s="153"/>
-      <c r="AU37" s="154"/>
-      <c r="AV37" s="149"/>
+      <c r="AF37" s="142"/>
+      <c r="AG37" s="144"/>
+      <c r="AH37" s="144"/>
+      <c r="AI37" s="134"/>
+      <c r="AJ37" s="118"/>
+      <c r="AK37" s="119"/>
+      <c r="AL37" s="119"/>
+      <c r="AM37" s="120"/>
+      <c r="AN37" s="145"/>
+      <c r="AO37" s="146"/>
+      <c r="AP37" s="146"/>
+      <c r="AQ37" s="120"/>
+      <c r="AR37" s="141"/>
+      <c r="AS37" s="141"/>
+      <c r="AT37" s="141"/>
+      <c r="AU37" s="142"/>
+      <c r="AV37" s="129"/>
       <c r="AW37" s="46"/>
     </row>
     <row r="38" spans="1:49" x14ac:dyDescent="0.2">
@@ -3568,23 +3624,23 @@
       <c r="AC38" s="36"/>
       <c r="AD38" s="36"/>
       <c r="AE38" s="42"/>
-      <c r="AF38" s="154"/>
-      <c r="AG38" s="168"/>
-      <c r="AH38" s="168"/>
-      <c r="AI38" s="165"/>
-      <c r="AJ38" s="119"/>
-      <c r="AK38" s="120"/>
-      <c r="AL38" s="120"/>
-      <c r="AM38" s="121"/>
-      <c r="AN38" s="158"/>
-      <c r="AO38" s="159"/>
-      <c r="AP38" s="159"/>
-      <c r="AQ38" s="121"/>
-      <c r="AR38" s="153"/>
-      <c r="AS38" s="153"/>
-      <c r="AT38" s="153"/>
-      <c r="AU38" s="154"/>
-      <c r="AV38" s="149"/>
+      <c r="AF38" s="142"/>
+      <c r="AG38" s="144"/>
+      <c r="AH38" s="144"/>
+      <c r="AI38" s="134"/>
+      <c r="AJ38" s="118"/>
+      <c r="AK38" s="119"/>
+      <c r="AL38" s="119"/>
+      <c r="AM38" s="120"/>
+      <c r="AN38" s="145"/>
+      <c r="AO38" s="146"/>
+      <c r="AP38" s="146"/>
+      <c r="AQ38" s="120"/>
+      <c r="AR38" s="141"/>
+      <c r="AS38" s="141"/>
+      <c r="AT38" s="141"/>
+      <c r="AU38" s="142"/>
+      <c r="AV38" s="129"/>
       <c r="AW38" s="46"/>
     </row>
     <row r="39" spans="1:49" x14ac:dyDescent="0.2">
@@ -3619,23 +3675,23 @@
       <c r="AC39" s="36"/>
       <c r="AD39" s="36"/>
       <c r="AE39" s="42"/>
-      <c r="AF39" s="154"/>
-      <c r="AG39" s="168"/>
-      <c r="AH39" s="168"/>
-      <c r="AI39" s="165"/>
-      <c r="AJ39" s="119"/>
-      <c r="AK39" s="120"/>
-      <c r="AL39" s="120"/>
-      <c r="AM39" s="121"/>
-      <c r="AN39" s="158"/>
-      <c r="AO39" s="159"/>
-      <c r="AP39" s="159"/>
-      <c r="AQ39" s="121"/>
-      <c r="AR39" s="130"/>
-      <c r="AS39" s="130"/>
-      <c r="AT39" s="130"/>
-      <c r="AU39" s="160"/>
-      <c r="AV39" s="150"/>
+      <c r="AF39" s="142"/>
+      <c r="AG39" s="144"/>
+      <c r="AH39" s="144"/>
+      <c r="AI39" s="134"/>
+      <c r="AJ39" s="118"/>
+      <c r="AK39" s="119"/>
+      <c r="AL39" s="119"/>
+      <c r="AM39" s="120"/>
+      <c r="AN39" s="145"/>
+      <c r="AO39" s="146"/>
+      <c r="AP39" s="146"/>
+      <c r="AQ39" s="120"/>
+      <c r="AR39" s="151"/>
+      <c r="AS39" s="151"/>
+      <c r="AT39" s="151"/>
+      <c r="AU39" s="152"/>
+      <c r="AV39" s="130"/>
       <c r="AW39" s="46"/>
     </row>
     <row r="40" spans="1:49" x14ac:dyDescent="0.2">
@@ -3670,23 +3726,23 @@
       <c r="AC40" s="36"/>
       <c r="AD40" s="36"/>
       <c r="AE40" s="42"/>
-      <c r="AF40" s="154"/>
-      <c r="AG40" s="168"/>
-      <c r="AH40" s="168"/>
-      <c r="AI40" s="165"/>
-      <c r="AJ40" s="119"/>
-      <c r="AK40" s="120"/>
-      <c r="AL40" s="120"/>
-      <c r="AM40" s="121"/>
-      <c r="AN40" s="158"/>
-      <c r="AO40" s="159"/>
-      <c r="AP40" s="159"/>
-      <c r="AQ40" s="121"/>
-      <c r="AR40" s="130"/>
-      <c r="AS40" s="130"/>
-      <c r="AT40" s="130"/>
-      <c r="AU40" s="160"/>
-      <c r="AV40" s="150"/>
+      <c r="AF40" s="142"/>
+      <c r="AG40" s="144"/>
+      <c r="AH40" s="144"/>
+      <c r="AI40" s="134"/>
+      <c r="AJ40" s="118"/>
+      <c r="AK40" s="119"/>
+      <c r="AL40" s="119"/>
+      <c r="AM40" s="120"/>
+      <c r="AN40" s="145"/>
+      <c r="AO40" s="146"/>
+      <c r="AP40" s="146"/>
+      <c r="AQ40" s="120"/>
+      <c r="AR40" s="151"/>
+      <c r="AS40" s="151"/>
+      <c r="AT40" s="151"/>
+      <c r="AU40" s="152"/>
+      <c r="AV40" s="130"/>
       <c r="AW40" s="46"/>
     </row>
     <row r="41" spans="1:49" x14ac:dyDescent="0.2">
@@ -3721,23 +3777,23 @@
       <c r="AC41" s="36"/>
       <c r="AD41" s="36"/>
       <c r="AE41" s="42"/>
-      <c r="AF41" s="154"/>
-      <c r="AG41" s="168"/>
-      <c r="AH41" s="168"/>
-      <c r="AI41" s="165"/>
-      <c r="AJ41" s="119"/>
-      <c r="AK41" s="120"/>
-      <c r="AL41" s="120"/>
-      <c r="AM41" s="121"/>
-      <c r="AN41" s="158"/>
-      <c r="AO41" s="159"/>
-      <c r="AP41" s="159"/>
-      <c r="AQ41" s="121"/>
-      <c r="AR41" s="130"/>
-      <c r="AS41" s="130"/>
-      <c r="AT41" s="130"/>
-      <c r="AU41" s="160"/>
-      <c r="AV41" s="150"/>
+      <c r="AF41" s="142"/>
+      <c r="AG41" s="144"/>
+      <c r="AH41" s="144"/>
+      <c r="AI41" s="134"/>
+      <c r="AJ41" s="118"/>
+      <c r="AK41" s="119"/>
+      <c r="AL41" s="119"/>
+      <c r="AM41" s="120"/>
+      <c r="AN41" s="145"/>
+      <c r="AO41" s="146"/>
+      <c r="AP41" s="146"/>
+      <c r="AQ41" s="120"/>
+      <c r="AR41" s="151"/>
+      <c r="AS41" s="151"/>
+      <c r="AT41" s="151"/>
+      <c r="AU41" s="152"/>
+      <c r="AV41" s="130"/>
       <c r="AW41" s="46"/>
     </row>
     <row r="42" spans="1:49" x14ac:dyDescent="0.2">
@@ -3772,23 +3828,23 @@
       <c r="AC42" s="36"/>
       <c r="AD42" s="36"/>
       <c r="AE42" s="42"/>
-      <c r="AF42" s="154"/>
-      <c r="AG42" s="168"/>
-      <c r="AH42" s="168"/>
-      <c r="AI42" s="165"/>
-      <c r="AJ42" s="119"/>
-      <c r="AK42" s="120"/>
-      <c r="AL42" s="120"/>
-      <c r="AM42" s="121"/>
-      <c r="AN42" s="158"/>
-      <c r="AO42" s="159"/>
-      <c r="AP42" s="159"/>
-      <c r="AQ42" s="121"/>
-      <c r="AR42" s="130"/>
-      <c r="AS42" s="130"/>
-      <c r="AT42" s="130"/>
-      <c r="AU42" s="160"/>
-      <c r="AV42" s="150"/>
+      <c r="AF42" s="142"/>
+      <c r="AG42" s="144"/>
+      <c r="AH42" s="144"/>
+      <c r="AI42" s="134"/>
+      <c r="AJ42" s="118"/>
+      <c r="AK42" s="119"/>
+      <c r="AL42" s="119"/>
+      <c r="AM42" s="120"/>
+      <c r="AN42" s="145"/>
+      <c r="AO42" s="146"/>
+      <c r="AP42" s="146"/>
+      <c r="AQ42" s="120"/>
+      <c r="AR42" s="151"/>
+      <c r="AS42" s="151"/>
+      <c r="AT42" s="151"/>
+      <c r="AU42" s="152"/>
+      <c r="AV42" s="130"/>
       <c r="AW42" s="46"/>
     </row>
     <row r="43" spans="1:49" x14ac:dyDescent="0.2">
@@ -3823,23 +3879,23 @@
       <c r="AC43" s="36"/>
       <c r="AD43" s="36"/>
       <c r="AE43" s="42"/>
-      <c r="AF43" s="154"/>
-      <c r="AG43" s="168"/>
-      <c r="AH43" s="168"/>
-      <c r="AI43" s="165"/>
-      <c r="AJ43" s="119"/>
-      <c r="AK43" s="120"/>
-      <c r="AL43" s="120"/>
-      <c r="AM43" s="121"/>
-      <c r="AN43" s="158"/>
-      <c r="AO43" s="159"/>
-      <c r="AP43" s="159"/>
-      <c r="AQ43" s="121"/>
-      <c r="AR43" s="130"/>
-      <c r="AS43" s="130"/>
-      <c r="AT43" s="130"/>
-      <c r="AU43" s="160"/>
-      <c r="AV43" s="150"/>
+      <c r="AF43" s="142"/>
+      <c r="AG43" s="144"/>
+      <c r="AH43" s="144"/>
+      <c r="AI43" s="134"/>
+      <c r="AJ43" s="118"/>
+      <c r="AK43" s="119"/>
+      <c r="AL43" s="119"/>
+      <c r="AM43" s="120"/>
+      <c r="AN43" s="145"/>
+      <c r="AO43" s="146"/>
+      <c r="AP43" s="146"/>
+      <c r="AQ43" s="120"/>
+      <c r="AR43" s="151"/>
+      <c r="AS43" s="151"/>
+      <c r="AT43" s="151"/>
+      <c r="AU43" s="152"/>
+      <c r="AV43" s="130"/>
       <c r="AW43" s="46"/>
     </row>
     <row r="44" spans="1:49" x14ac:dyDescent="0.2">
@@ -3874,23 +3930,23 @@
       <c r="AC44" s="36"/>
       <c r="AD44" s="36"/>
       <c r="AE44" s="42"/>
-      <c r="AF44" s="154"/>
-      <c r="AG44" s="168"/>
-      <c r="AH44" s="168"/>
-      <c r="AI44" s="165"/>
-      <c r="AJ44" s="119"/>
-      <c r="AK44" s="120"/>
-      <c r="AL44" s="120"/>
-      <c r="AM44" s="121"/>
-      <c r="AN44" s="158"/>
-      <c r="AO44" s="159"/>
-      <c r="AP44" s="159"/>
-      <c r="AQ44" s="121"/>
-      <c r="AR44" s="130"/>
-      <c r="AS44" s="130"/>
-      <c r="AT44" s="130"/>
-      <c r="AU44" s="160"/>
-      <c r="AV44" s="150"/>
+      <c r="AF44" s="142"/>
+      <c r="AG44" s="144"/>
+      <c r="AH44" s="144"/>
+      <c r="AI44" s="134"/>
+      <c r="AJ44" s="118"/>
+      <c r="AK44" s="119"/>
+      <c r="AL44" s="119"/>
+      <c r="AM44" s="120"/>
+      <c r="AN44" s="145"/>
+      <c r="AO44" s="146"/>
+      <c r="AP44" s="146"/>
+      <c r="AQ44" s="120"/>
+      <c r="AR44" s="151"/>
+      <c r="AS44" s="151"/>
+      <c r="AT44" s="151"/>
+      <c r="AU44" s="152"/>
+      <c r="AV44" s="130"/>
       <c r="AW44" s="46"/>
     </row>
     <row r="45" spans="1:49" x14ac:dyDescent="0.2">
@@ -3925,23 +3981,23 @@
       <c r="AC45" s="36"/>
       <c r="AD45" s="36"/>
       <c r="AE45" s="42"/>
-      <c r="AF45" s="154"/>
-      <c r="AG45" s="168"/>
-      <c r="AH45" s="168"/>
-      <c r="AI45" s="165"/>
-      <c r="AJ45" s="119"/>
-      <c r="AK45" s="120"/>
-      <c r="AL45" s="120"/>
-      <c r="AM45" s="121"/>
-      <c r="AN45" s="158"/>
-      <c r="AO45" s="159"/>
-      <c r="AP45" s="159"/>
-      <c r="AQ45" s="121"/>
-      <c r="AR45" s="130"/>
-      <c r="AS45" s="130"/>
-      <c r="AT45" s="130"/>
-      <c r="AU45" s="160"/>
-      <c r="AV45" s="150"/>
+      <c r="AF45" s="142"/>
+      <c r="AG45" s="144"/>
+      <c r="AH45" s="144"/>
+      <c r="AI45" s="134"/>
+      <c r="AJ45" s="118"/>
+      <c r="AK45" s="119"/>
+      <c r="AL45" s="119"/>
+      <c r="AM45" s="120"/>
+      <c r="AN45" s="145"/>
+      <c r="AO45" s="146"/>
+      <c r="AP45" s="146"/>
+      <c r="AQ45" s="120"/>
+      <c r="AR45" s="151"/>
+      <c r="AS45" s="151"/>
+      <c r="AT45" s="151"/>
+      <c r="AU45" s="152"/>
+      <c r="AV45" s="130"/>
       <c r="AW45" s="46"/>
     </row>
     <row r="46" spans="1:49" x14ac:dyDescent="0.2">
@@ -3976,23 +4032,23 @@
       <c r="AC46" s="36"/>
       <c r="AD46" s="36"/>
       <c r="AE46" s="42"/>
-      <c r="AF46" s="154"/>
-      <c r="AG46" s="168"/>
-      <c r="AH46" s="168"/>
-      <c r="AI46" s="165"/>
-      <c r="AJ46" s="119"/>
-      <c r="AK46" s="120"/>
-      <c r="AL46" s="120"/>
-      <c r="AM46" s="121"/>
-      <c r="AN46" s="158"/>
-      <c r="AO46" s="159"/>
-      <c r="AP46" s="159"/>
-      <c r="AQ46" s="121"/>
-      <c r="AR46" s="130"/>
-      <c r="AS46" s="130"/>
-      <c r="AT46" s="130"/>
-      <c r="AU46" s="160"/>
-      <c r="AV46" s="150"/>
+      <c r="AF46" s="142"/>
+      <c r="AG46" s="144"/>
+      <c r="AH46" s="144"/>
+      <c r="AI46" s="134"/>
+      <c r="AJ46" s="118"/>
+      <c r="AK46" s="119"/>
+      <c r="AL46" s="119"/>
+      <c r="AM46" s="120"/>
+      <c r="AN46" s="145"/>
+      <c r="AO46" s="146"/>
+      <c r="AP46" s="146"/>
+      <c r="AQ46" s="120"/>
+      <c r="AR46" s="151"/>
+      <c r="AS46" s="151"/>
+      <c r="AT46" s="151"/>
+      <c r="AU46" s="152"/>
+      <c r="AV46" s="130"/>
       <c r="AW46" s="46"/>
     </row>
     <row r="47" spans="1:49" x14ac:dyDescent="0.2">
@@ -4027,23 +4083,23 @@
       <c r="AC47" s="36"/>
       <c r="AD47" s="36"/>
       <c r="AE47" s="42"/>
-      <c r="AF47" s="154"/>
-      <c r="AG47" s="168"/>
-      <c r="AH47" s="168"/>
-      <c r="AI47" s="165"/>
-      <c r="AJ47" s="119"/>
-      <c r="AK47" s="120"/>
-      <c r="AL47" s="120"/>
-      <c r="AM47" s="121"/>
-      <c r="AN47" s="158"/>
-      <c r="AO47" s="159"/>
-      <c r="AP47" s="159"/>
-      <c r="AQ47" s="121"/>
-      <c r="AR47" s="130"/>
-      <c r="AS47" s="130"/>
-      <c r="AT47" s="130"/>
-      <c r="AU47" s="160"/>
-      <c r="AV47" s="150"/>
+      <c r="AF47" s="142"/>
+      <c r="AG47" s="144"/>
+      <c r="AH47" s="144"/>
+      <c r="AI47" s="134"/>
+      <c r="AJ47" s="118"/>
+      <c r="AK47" s="119"/>
+      <c r="AL47" s="119"/>
+      <c r="AM47" s="120"/>
+      <c r="AN47" s="145"/>
+      <c r="AO47" s="146"/>
+      <c r="AP47" s="146"/>
+      <c r="AQ47" s="120"/>
+      <c r="AR47" s="151"/>
+      <c r="AS47" s="151"/>
+      <c r="AT47" s="151"/>
+      <c r="AU47" s="152"/>
+      <c r="AV47" s="130"/>
       <c r="AW47" s="46"/>
     </row>
     <row r="48" spans="1:49" x14ac:dyDescent="0.2">
@@ -4078,23 +4134,23 @@
       <c r="AC48" s="36"/>
       <c r="AD48" s="36"/>
       <c r="AE48" s="42"/>
-      <c r="AF48" s="154"/>
-      <c r="AG48" s="168"/>
-      <c r="AH48" s="168"/>
-      <c r="AI48" s="165"/>
-      <c r="AJ48" s="119"/>
-      <c r="AK48" s="120"/>
-      <c r="AL48" s="120"/>
-      <c r="AM48" s="121"/>
-      <c r="AN48" s="158"/>
-      <c r="AO48" s="159"/>
-      <c r="AP48" s="159"/>
-      <c r="AQ48" s="121"/>
-      <c r="AR48" s="130"/>
-      <c r="AS48" s="130"/>
-      <c r="AT48" s="130"/>
-      <c r="AU48" s="160"/>
-      <c r="AV48" s="150"/>
+      <c r="AF48" s="142"/>
+      <c r="AG48" s="144"/>
+      <c r="AH48" s="144"/>
+      <c r="AI48" s="134"/>
+      <c r="AJ48" s="118"/>
+      <c r="AK48" s="119"/>
+      <c r="AL48" s="119"/>
+      <c r="AM48" s="120"/>
+      <c r="AN48" s="145"/>
+      <c r="AO48" s="146"/>
+      <c r="AP48" s="146"/>
+      <c r="AQ48" s="120"/>
+      <c r="AR48" s="151"/>
+      <c r="AS48" s="151"/>
+      <c r="AT48" s="151"/>
+      <c r="AU48" s="152"/>
+      <c r="AV48" s="130"/>
       <c r="AW48" s="46"/>
     </row>
     <row r="49" spans="1:54" x14ac:dyDescent="0.2">
@@ -4129,23 +4185,23 @@
       <c r="AC49" s="36"/>
       <c r="AD49" s="36"/>
       <c r="AE49" s="42"/>
-      <c r="AF49" s="154"/>
-      <c r="AG49" s="168"/>
-      <c r="AH49" s="168"/>
-      <c r="AI49" s="165"/>
-      <c r="AJ49" s="119"/>
-      <c r="AK49" s="120"/>
-      <c r="AL49" s="120"/>
-      <c r="AM49" s="121"/>
-      <c r="AN49" s="158"/>
-      <c r="AO49" s="159"/>
-      <c r="AP49" s="159"/>
-      <c r="AQ49" s="121"/>
-      <c r="AR49" s="130"/>
-      <c r="AS49" s="130"/>
-      <c r="AT49" s="130"/>
-      <c r="AU49" s="160"/>
-      <c r="AV49" s="150"/>
+      <c r="AF49" s="142"/>
+      <c r="AG49" s="144"/>
+      <c r="AH49" s="144"/>
+      <c r="AI49" s="134"/>
+      <c r="AJ49" s="118"/>
+      <c r="AK49" s="119"/>
+      <c r="AL49" s="119"/>
+      <c r="AM49" s="120"/>
+      <c r="AN49" s="145"/>
+      <c r="AO49" s="146"/>
+      <c r="AP49" s="146"/>
+      <c r="AQ49" s="120"/>
+      <c r="AR49" s="151"/>
+      <c r="AS49" s="151"/>
+      <c r="AT49" s="151"/>
+      <c r="AU49" s="152"/>
+      <c r="AV49" s="130"/>
       <c r="AW49" s="46"/>
     </row>
     <row r="50" spans="1:54" x14ac:dyDescent="0.2">
@@ -4180,23 +4236,23 @@
       <c r="AC50" s="36"/>
       <c r="AD50" s="36"/>
       <c r="AE50" s="42"/>
-      <c r="AF50" s="154"/>
-      <c r="AG50" s="168"/>
-      <c r="AH50" s="168"/>
-      <c r="AI50" s="165"/>
-      <c r="AJ50" s="119"/>
-      <c r="AK50" s="120"/>
-      <c r="AL50" s="120"/>
-      <c r="AM50" s="121"/>
-      <c r="AN50" s="158"/>
-      <c r="AO50" s="159"/>
-      <c r="AP50" s="159"/>
-      <c r="AQ50" s="121"/>
-      <c r="AR50" s="130"/>
-      <c r="AS50" s="130"/>
-      <c r="AT50" s="130"/>
-      <c r="AU50" s="160"/>
-      <c r="AV50" s="150"/>
+      <c r="AF50" s="142"/>
+      <c r="AG50" s="144"/>
+      <c r="AH50" s="144"/>
+      <c r="AI50" s="134"/>
+      <c r="AJ50" s="118"/>
+      <c r="AK50" s="119"/>
+      <c r="AL50" s="119"/>
+      <c r="AM50" s="120"/>
+      <c r="AN50" s="145"/>
+      <c r="AO50" s="146"/>
+      <c r="AP50" s="146"/>
+      <c r="AQ50" s="120"/>
+      <c r="AR50" s="151"/>
+      <c r="AS50" s="151"/>
+      <c r="AT50" s="151"/>
+      <c r="AU50" s="152"/>
+      <c r="AV50" s="130"/>
       <c r="AW50" s="46"/>
     </row>
     <row r="51" spans="1:54" x14ac:dyDescent="0.2">
@@ -4231,23 +4287,23 @@
       <c r="AC51" s="36"/>
       <c r="AD51" s="36"/>
       <c r="AE51" s="42"/>
-      <c r="AF51" s="154"/>
-      <c r="AG51" s="168"/>
-      <c r="AH51" s="168"/>
-      <c r="AI51" s="165"/>
-      <c r="AJ51" s="119"/>
-      <c r="AK51" s="120"/>
-      <c r="AL51" s="120"/>
-      <c r="AM51" s="121"/>
-      <c r="AN51" s="158"/>
-      <c r="AO51" s="159"/>
-      <c r="AP51" s="159"/>
-      <c r="AQ51" s="121"/>
-      <c r="AR51" s="130"/>
-      <c r="AS51" s="130"/>
-      <c r="AT51" s="130"/>
-      <c r="AU51" s="160"/>
-      <c r="AV51" s="150"/>
+      <c r="AF51" s="142"/>
+      <c r="AG51" s="144"/>
+      <c r="AH51" s="144"/>
+      <c r="AI51" s="134"/>
+      <c r="AJ51" s="118"/>
+      <c r="AK51" s="119"/>
+      <c r="AL51" s="119"/>
+      <c r="AM51" s="120"/>
+      <c r="AN51" s="145"/>
+      <c r="AO51" s="146"/>
+      <c r="AP51" s="146"/>
+      <c r="AQ51" s="120"/>
+      <c r="AR51" s="151"/>
+      <c r="AS51" s="151"/>
+      <c r="AT51" s="151"/>
+      <c r="AU51" s="152"/>
+      <c r="AV51" s="130"/>
       <c r="AW51" s="46"/>
     </row>
     <row r="52" spans="1:54" x14ac:dyDescent="0.2">
@@ -4282,23 +4338,23 @@
       <c r="AC52" s="36"/>
       <c r="AD52" s="36"/>
       <c r="AE52" s="42"/>
-      <c r="AF52" s="154"/>
-      <c r="AG52" s="168"/>
-      <c r="AH52" s="168"/>
-      <c r="AI52" s="165"/>
-      <c r="AJ52" s="119"/>
-      <c r="AK52" s="120"/>
-      <c r="AL52" s="120"/>
-      <c r="AM52" s="121"/>
-      <c r="AN52" s="158"/>
-      <c r="AO52" s="159"/>
-      <c r="AP52" s="159"/>
-      <c r="AQ52" s="121"/>
-      <c r="AR52" s="130"/>
-      <c r="AS52" s="130"/>
-      <c r="AT52" s="130"/>
-      <c r="AU52" s="160"/>
-      <c r="AV52" s="150"/>
+      <c r="AF52" s="142"/>
+      <c r="AG52" s="144"/>
+      <c r="AH52" s="144"/>
+      <c r="AI52" s="134"/>
+      <c r="AJ52" s="118"/>
+      <c r="AK52" s="119"/>
+      <c r="AL52" s="119"/>
+      <c r="AM52" s="120"/>
+      <c r="AN52" s="145"/>
+      <c r="AO52" s="146"/>
+      <c r="AP52" s="146"/>
+      <c r="AQ52" s="120"/>
+      <c r="AR52" s="151"/>
+      <c r="AS52" s="151"/>
+      <c r="AT52" s="151"/>
+      <c r="AU52" s="152"/>
+      <c r="AV52" s="130"/>
       <c r="AW52" s="46"/>
     </row>
     <row r="53" spans="1:54" x14ac:dyDescent="0.2">
@@ -4333,23 +4389,23 @@
       <c r="AC53" s="36"/>
       <c r="AD53" s="36"/>
       <c r="AE53" s="42"/>
-      <c r="AF53" s="154"/>
-      <c r="AG53" s="168"/>
-      <c r="AH53" s="168"/>
-      <c r="AI53" s="165"/>
-      <c r="AJ53" s="119"/>
-      <c r="AK53" s="120"/>
-      <c r="AL53" s="120"/>
-      <c r="AM53" s="121"/>
-      <c r="AN53" s="158"/>
-      <c r="AO53" s="159"/>
-      <c r="AP53" s="159"/>
-      <c r="AQ53" s="121"/>
-      <c r="AR53" s="130"/>
-      <c r="AS53" s="130"/>
-      <c r="AT53" s="130"/>
-      <c r="AU53" s="160"/>
-      <c r="AV53" s="150"/>
+      <c r="AF53" s="142"/>
+      <c r="AG53" s="144"/>
+      <c r="AH53" s="144"/>
+      <c r="AI53" s="134"/>
+      <c r="AJ53" s="118"/>
+      <c r="AK53" s="119"/>
+      <c r="AL53" s="119"/>
+      <c r="AM53" s="120"/>
+      <c r="AN53" s="145"/>
+      <c r="AO53" s="146"/>
+      <c r="AP53" s="146"/>
+      <c r="AQ53" s="120"/>
+      <c r="AR53" s="151"/>
+      <c r="AS53" s="151"/>
+      <c r="AT53" s="151"/>
+      <c r="AU53" s="152"/>
+      <c r="AV53" s="130"/>
       <c r="AW53" s="46"/>
     </row>
     <row r="54" spans="1:54" x14ac:dyDescent="0.2">
@@ -4384,23 +4440,23 @@
       <c r="AC54" s="36"/>
       <c r="AD54" s="36"/>
       <c r="AE54" s="42"/>
-      <c r="AF54" s="154"/>
-      <c r="AG54" s="168"/>
-      <c r="AH54" s="168"/>
-      <c r="AI54" s="165"/>
-      <c r="AJ54" s="119"/>
-      <c r="AK54" s="120"/>
-      <c r="AL54" s="120"/>
-      <c r="AM54" s="121"/>
-      <c r="AN54" s="158"/>
-      <c r="AO54" s="159"/>
-      <c r="AP54" s="159"/>
-      <c r="AQ54" s="121"/>
-      <c r="AR54" s="130"/>
-      <c r="AS54" s="130"/>
-      <c r="AT54" s="130"/>
-      <c r="AU54" s="160"/>
-      <c r="AV54" s="150"/>
+      <c r="AF54" s="142"/>
+      <c r="AG54" s="144"/>
+      <c r="AH54" s="144"/>
+      <c r="AI54" s="134"/>
+      <c r="AJ54" s="118"/>
+      <c r="AK54" s="119"/>
+      <c r="AL54" s="119"/>
+      <c r="AM54" s="120"/>
+      <c r="AN54" s="145"/>
+      <c r="AO54" s="146"/>
+      <c r="AP54" s="146"/>
+      <c r="AQ54" s="120"/>
+      <c r="AR54" s="151"/>
+      <c r="AS54" s="151"/>
+      <c r="AT54" s="151"/>
+      <c r="AU54" s="152"/>
+      <c r="AV54" s="130"/>
       <c r="AW54" s="46"/>
     </row>
     <row r="55" spans="1:54" x14ac:dyDescent="0.2">
@@ -4435,23 +4491,23 @@
       <c r="AC55" s="36"/>
       <c r="AD55" s="36"/>
       <c r="AE55" s="42"/>
-      <c r="AF55" s="154"/>
-      <c r="AG55" s="168"/>
-      <c r="AH55" s="168"/>
-      <c r="AI55" s="165"/>
-      <c r="AJ55" s="119"/>
-      <c r="AK55" s="120"/>
-      <c r="AL55" s="120"/>
-      <c r="AM55" s="121"/>
-      <c r="AN55" s="158"/>
-      <c r="AO55" s="159"/>
-      <c r="AP55" s="159"/>
-      <c r="AQ55" s="121"/>
-      <c r="AR55" s="130"/>
-      <c r="AS55" s="130"/>
-      <c r="AT55" s="130"/>
-      <c r="AU55" s="160"/>
-      <c r="AV55" s="150"/>
+      <c r="AF55" s="142"/>
+      <c r="AG55" s="144"/>
+      <c r="AH55" s="144"/>
+      <c r="AI55" s="134"/>
+      <c r="AJ55" s="118"/>
+      <c r="AK55" s="119"/>
+      <c r="AL55" s="119"/>
+      <c r="AM55" s="120"/>
+      <c r="AN55" s="145"/>
+      <c r="AO55" s="146"/>
+      <c r="AP55" s="146"/>
+      <c r="AQ55" s="120"/>
+      <c r="AR55" s="151"/>
+      <c r="AS55" s="151"/>
+      <c r="AT55" s="151"/>
+      <c r="AU55" s="152"/>
+      <c r="AV55" s="130"/>
       <c r="AW55" s="46"/>
     </row>
     <row r="56" spans="1:54" x14ac:dyDescent="0.2">
@@ -4486,23 +4542,23 @@
       <c r="AC56" s="36"/>
       <c r="AD56" s="36"/>
       <c r="AE56" s="42"/>
-      <c r="AF56" s="154"/>
-      <c r="AG56" s="168"/>
-      <c r="AH56" s="168"/>
-      <c r="AI56" s="165"/>
-      <c r="AJ56" s="119"/>
-      <c r="AK56" s="120"/>
-      <c r="AL56" s="120"/>
-      <c r="AM56" s="121"/>
-      <c r="AN56" s="158"/>
-      <c r="AO56" s="159"/>
-      <c r="AP56" s="159"/>
-      <c r="AQ56" s="121"/>
-      <c r="AR56" s="130"/>
-      <c r="AS56" s="130"/>
-      <c r="AT56" s="130"/>
-      <c r="AU56" s="160"/>
-      <c r="AV56" s="150"/>
+      <c r="AF56" s="142"/>
+      <c r="AG56" s="144"/>
+      <c r="AH56" s="144"/>
+      <c r="AI56" s="134"/>
+      <c r="AJ56" s="118"/>
+      <c r="AK56" s="119"/>
+      <c r="AL56" s="119"/>
+      <c r="AM56" s="120"/>
+      <c r="AN56" s="145"/>
+      <c r="AO56" s="146"/>
+      <c r="AP56" s="146"/>
+      <c r="AQ56" s="120"/>
+      <c r="AR56" s="151"/>
+      <c r="AS56" s="151"/>
+      <c r="AT56" s="151"/>
+      <c r="AU56" s="152"/>
+      <c r="AV56" s="130"/>
       <c r="AW56" s="46"/>
     </row>
     <row r="57" spans="1:54" x14ac:dyDescent="0.2">
@@ -4537,23 +4593,23 @@
       <c r="AC57" s="36"/>
       <c r="AD57" s="36"/>
       <c r="AE57" s="42"/>
-      <c r="AF57" s="154"/>
-      <c r="AG57" s="168"/>
-      <c r="AH57" s="168"/>
-      <c r="AI57" s="165"/>
-      <c r="AJ57" s="119"/>
-      <c r="AK57" s="120"/>
-      <c r="AL57" s="120"/>
-      <c r="AM57" s="121"/>
-      <c r="AN57" s="158"/>
-      <c r="AO57" s="159"/>
-      <c r="AP57" s="159"/>
-      <c r="AQ57" s="121"/>
-      <c r="AR57" s="130"/>
-      <c r="AS57" s="130"/>
-      <c r="AT57" s="130"/>
-      <c r="AU57" s="160"/>
-      <c r="AV57" s="150"/>
+      <c r="AF57" s="142"/>
+      <c r="AG57" s="144"/>
+      <c r="AH57" s="144"/>
+      <c r="AI57" s="134"/>
+      <c r="AJ57" s="118"/>
+      <c r="AK57" s="119"/>
+      <c r="AL57" s="119"/>
+      <c r="AM57" s="120"/>
+      <c r="AN57" s="145"/>
+      <c r="AO57" s="146"/>
+      <c r="AP57" s="146"/>
+      <c r="AQ57" s="120"/>
+      <c r="AR57" s="151"/>
+      <c r="AS57" s="151"/>
+      <c r="AT57" s="151"/>
+      <c r="AU57" s="152"/>
+      <c r="AV57" s="130"/>
       <c r="AW57" s="46"/>
     </row>
     <row r="58" spans="1:54" x14ac:dyDescent="0.2">
@@ -4588,23 +4644,23 @@
       <c r="AC58" s="36"/>
       <c r="AD58" s="36"/>
       <c r="AE58" s="42"/>
-      <c r="AF58" s="154"/>
-      <c r="AG58" s="168"/>
-      <c r="AH58" s="168"/>
-      <c r="AI58" s="165"/>
-      <c r="AJ58" s="119"/>
-      <c r="AK58" s="120"/>
-      <c r="AL58" s="120"/>
-      <c r="AM58" s="121"/>
-      <c r="AN58" s="158"/>
-      <c r="AO58" s="159"/>
-      <c r="AP58" s="159"/>
-      <c r="AQ58" s="121"/>
-      <c r="AR58" s="130"/>
-      <c r="AS58" s="130"/>
-      <c r="AT58" s="130"/>
-      <c r="AU58" s="160"/>
-      <c r="AV58" s="150"/>
+      <c r="AF58" s="142"/>
+      <c r="AG58" s="144"/>
+      <c r="AH58" s="144"/>
+      <c r="AI58" s="134"/>
+      <c r="AJ58" s="118"/>
+      <c r="AK58" s="119"/>
+      <c r="AL58" s="119"/>
+      <c r="AM58" s="120"/>
+      <c r="AN58" s="145"/>
+      <c r="AO58" s="146"/>
+      <c r="AP58" s="146"/>
+      <c r="AQ58" s="120"/>
+      <c r="AR58" s="151"/>
+      <c r="AS58" s="151"/>
+      <c r="AT58" s="151"/>
+      <c r="AU58" s="152"/>
+      <c r="AV58" s="130"/>
       <c r="AW58" s="46"/>
     </row>
     <row r="59" spans="1:54" x14ac:dyDescent="0.2">
@@ -4639,23 +4695,23 @@
       <c r="AC59" s="36"/>
       <c r="AD59" s="36"/>
       <c r="AE59" s="42"/>
-      <c r="AF59" s="154"/>
-      <c r="AG59" s="168"/>
-      <c r="AH59" s="168"/>
-      <c r="AI59" s="165"/>
-      <c r="AJ59" s="119"/>
-      <c r="AK59" s="120"/>
-      <c r="AL59" s="120"/>
-      <c r="AM59" s="121"/>
-      <c r="AN59" s="158"/>
-      <c r="AO59" s="159"/>
-      <c r="AP59" s="159"/>
-      <c r="AQ59" s="121"/>
-      <c r="AR59" s="130"/>
-      <c r="AS59" s="130"/>
-      <c r="AT59" s="130"/>
-      <c r="AU59" s="160"/>
-      <c r="AV59" s="150"/>
+      <c r="AF59" s="142"/>
+      <c r="AG59" s="144"/>
+      <c r="AH59" s="144"/>
+      <c r="AI59" s="134"/>
+      <c r="AJ59" s="118"/>
+      <c r="AK59" s="119"/>
+      <c r="AL59" s="119"/>
+      <c r="AM59" s="120"/>
+      <c r="AN59" s="145"/>
+      <c r="AO59" s="146"/>
+      <c r="AP59" s="146"/>
+      <c r="AQ59" s="120"/>
+      <c r="AR59" s="151"/>
+      <c r="AS59" s="151"/>
+      <c r="AT59" s="151"/>
+      <c r="AU59" s="152"/>
+      <c r="AV59" s="130"/>
       <c r="AW59" s="46"/>
     </row>
     <row r="60" spans="1:54" x14ac:dyDescent="0.2">
@@ -4690,23 +4746,23 @@
       <c r="AC60" s="36"/>
       <c r="AD60" s="36"/>
       <c r="AE60" s="42"/>
-      <c r="AF60" s="154"/>
-      <c r="AG60" s="168"/>
-      <c r="AH60" s="168"/>
-      <c r="AI60" s="165"/>
-      <c r="AJ60" s="119"/>
-      <c r="AK60" s="120"/>
-      <c r="AL60" s="120"/>
-      <c r="AM60" s="121"/>
-      <c r="AN60" s="158"/>
-      <c r="AO60" s="159"/>
-      <c r="AP60" s="159"/>
-      <c r="AQ60" s="121"/>
-      <c r="AR60" s="130"/>
-      <c r="AS60" s="130"/>
-      <c r="AT60" s="130"/>
-      <c r="AU60" s="160"/>
-      <c r="AV60" s="150"/>
+      <c r="AF60" s="142"/>
+      <c r="AG60" s="144"/>
+      <c r="AH60" s="144"/>
+      <c r="AI60" s="134"/>
+      <c r="AJ60" s="118"/>
+      <c r="AK60" s="119"/>
+      <c r="AL60" s="119"/>
+      <c r="AM60" s="120"/>
+      <c r="AN60" s="145"/>
+      <c r="AO60" s="146"/>
+      <c r="AP60" s="146"/>
+      <c r="AQ60" s="120"/>
+      <c r="AR60" s="151"/>
+      <c r="AS60" s="151"/>
+      <c r="AT60" s="151"/>
+      <c r="AU60" s="152"/>
+      <c r="AV60" s="130"/>
       <c r="AW60" s="46"/>
     </row>
     <row r="61" spans="1:54" x14ac:dyDescent="0.2">
@@ -4741,24 +4797,24 @@
       <c r="AC61" s="36"/>
       <c r="AD61" s="36"/>
       <c r="AE61" s="42"/>
-      <c r="AF61" s="169"/>
-      <c r="AG61" s="170"/>
-      <c r="AH61" s="170"/>
-      <c r="AI61" s="166"/>
-      <c r="AJ61" s="125"/>
+      <c r="AF61" s="158"/>
+      <c r="AG61" s="159"/>
+      <c r="AH61" s="159"/>
+      <c r="AI61" s="135"/>
+      <c r="AJ61" s="124"/>
       <c r="AK61" s="52"/>
       <c r="AL61" s="52"/>
-      <c r="AM61" s="126"/>
-      <c r="AN61" s="161"/>
-      <c r="AO61" s="162"/>
-      <c r="AP61" s="162"/>
-      <c r="AQ61" s="126"/>
-      <c r="AR61" s="163"/>
-      <c r="AS61" s="164"/>
-      <c r="AT61" s="164"/>
-      <c r="AU61" s="164"/>
-      <c r="AV61" s="145"/>
-      <c r="AW61" s="86"/>
+      <c r="AM61" s="125"/>
+      <c r="AN61" s="156"/>
+      <c r="AO61" s="157"/>
+      <c r="AP61" s="157"/>
+      <c r="AQ61" s="125"/>
+      <c r="AR61" s="132"/>
+      <c r="AS61" s="133"/>
+      <c r="AT61" s="133"/>
+      <c r="AU61" s="133"/>
+      <c r="AV61" s="126"/>
+      <c r="AW61" s="85"/>
       <c r="AX61" s="33">
         <v>0.8</v>
       </c>
@@ -4812,21 +4868,21 @@
       <c r="AK62" s="55"/>
       <c r="AL62" s="55"/>
       <c r="AM62" s="55"/>
-      <c r="AN62" s="117"/>
-      <c r="AO62" s="117"/>
-      <c r="AP62" s="117" t="s">
+      <c r="AN62" s="116"/>
+      <c r="AO62" s="116"/>
+      <c r="AP62" s="116" t="s">
         <v>71</v>
       </c>
-      <c r="AQ62" s="117"/>
-      <c r="AR62" s="152">
+      <c r="AQ62" s="116"/>
+      <c r="AR62" s="160">
         <f>SUM(AR18:AU61)</f>
         <v>0</v>
       </c>
-      <c r="AS62" s="152"/>
-      <c r="AT62" s="152"/>
-      <c r="AU62" s="152"/>
-      <c r="AV62" s="118"/>
-      <c r="AW62" s="85"/>
+      <c r="AS62" s="160"/>
+      <c r="AT62" s="160"/>
+      <c r="AU62" s="160"/>
+      <c r="AV62" s="117"/>
+      <c r="AW62" s="84"/>
       <c r="AX62" s="32">
         <f>+AR62*AX61</f>
         <v>0</v>
@@ -4849,11 +4905,11 @@
       </c>
     </row>
     <row r="63" spans="1:54" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A63" s="98" t="s">
+      <c r="A63" s="97" t="s">
         <v>93</v>
       </c>
       <c r="B63" s="38"/>
-      <c r="C63" s="80" t="s">
+      <c r="C63" s="79" t="s">
         <v>121</v>
       </c>
       <c r="D63" s="38"/>
@@ -4965,7 +5021,7 @@
       <c r="E65" s="39"/>
       <c r="F65" s="39"/>
       <c r="G65" s="39"/>
-      <c r="H65" s="74"/>
+      <c r="H65" s="73"/>
       <c r="I65" s="36"/>
       <c r="J65" s="36"/>
       <c r="K65" s="36"/>
@@ -5113,14 +5169,14 @@
         <v>71</v>
       </c>
       <c r="AQ67" s="3"/>
-      <c r="AR67" s="133">
+      <c r="AR67" s="153">
         <f>0.7%*AR62</f>
         <v>0</v>
       </c>
-      <c r="AS67" s="134"/>
-      <c r="AT67" s="134"/>
-      <c r="AU67" s="146"/>
-      <c r="AV67" s="151"/>
+      <c r="AS67" s="154"/>
+      <c r="AT67" s="154"/>
+      <c r="AU67" s="155"/>
+      <c r="AV67" s="131"/>
       <c r="AW67" s="46"/>
     </row>
     <row r="68" spans="1:49" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5205,8 +5261,8 @@
       <c r="V69" s="39"/>
       <c r="W69" s="39"/>
       <c r="X69" s="39"/>
-      <c r="Y69" s="131"/>
-      <c r="Z69" s="132"/>
+      <c r="Y69" s="137"/>
+      <c r="Z69" s="147"/>
       <c r="AA69" s="36"/>
       <c r="AB69" s="36"/>
       <c r="AC69" s="36"/>
@@ -5764,7 +5820,7 @@
       <c r="D80" s="39"/>
       <c r="E80" s="39"/>
       <c r="F80" s="39"/>
-      <c r="G80" s="74"/>
+      <c r="G80" s="73"/>
       <c r="H80" s="39"/>
       <c r="I80" s="39"/>
       <c r="J80" s="39"/>
@@ -5780,13 +5836,13 @@
       <c r="R80" s="39"/>
       <c r="S80" s="39"/>
       <c r="T80" s="39"/>
-      <c r="U80" s="135"/>
-      <c r="V80" s="135"/>
-      <c r="W80" s="135"/>
-      <c r="X80" s="135"/>
-      <c r="Y80" s="135"/>
-      <c r="Z80" s="135"/>
-      <c r="AA80" s="135"/>
+      <c r="U80" s="161"/>
+      <c r="V80" s="161"/>
+      <c r="W80" s="161"/>
+      <c r="X80" s="161"/>
+      <c r="Y80" s="161"/>
+      <c r="Z80" s="161"/>
+      <c r="AA80" s="161"/>
       <c r="AB80" s="39"/>
       <c r="AC80" s="39"/>
       <c r="AD80" s="39"/>
@@ -5797,7 +5853,7 @@
       </c>
       <c r="AH80" s="39"/>
       <c r="AI80" s="39"/>
-      <c r="AJ80" s="76"/>
+      <c r="AJ80" s="75"/>
       <c r="AK80" s="39"/>
       <c r="AL80" s="39"/>
       <c r="AM80" s="39"/>
@@ -5872,7 +5928,7 @@
       <c r="F82" s="39"/>
       <c r="G82" s="39"/>
       <c r="H82" s="14"/>
-      <c r="I82" s="171" t="s">
+      <c r="I82" s="136" t="s">
         <v>81</v>
       </c>
       <c r="J82" s="39"/>
@@ -6264,16 +6320,16 @@
       <c r="AG89" s="2"/>
       <c r="AH89" s="36"/>
       <c r="AI89" s="36"/>
-      <c r="AJ89" s="132"/>
-      <c r="AK89" s="132"/>
-      <c r="AL89" s="132"/>
-      <c r="AM89" s="132"/>
-      <c r="AN89" s="132"/>
-      <c r="AO89" s="132"/>
-      <c r="AP89" s="132"/>
-      <c r="AQ89" s="132"/>
-      <c r="AR89" s="132"/>
-      <c r="AS89" s="132"/>
+      <c r="AJ89" s="147"/>
+      <c r="AK89" s="147"/>
+      <c r="AL89" s="147"/>
+      <c r="AM89" s="147"/>
+      <c r="AN89" s="147"/>
+      <c r="AO89" s="147"/>
+      <c r="AP89" s="147"/>
+      <c r="AQ89" s="147"/>
+      <c r="AR89" s="147"/>
+      <c r="AS89" s="147"/>
       <c r="AT89" s="36"/>
       <c r="AU89" s="36"/>
       <c r="AV89" s="42"/>
@@ -6335,62 +6391,7 @@
       <c r="N91" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="142">
-    <mergeCell ref="AF46:AH46"/>
-    <mergeCell ref="AF47:AH47"/>
-    <mergeCell ref="AF48:AH48"/>
-    <mergeCell ref="AF49:AH49"/>
-    <mergeCell ref="AF50:AH50"/>
-    <mergeCell ref="AF41:AH41"/>
-    <mergeCell ref="AF42:AH42"/>
-    <mergeCell ref="AF43:AH43"/>
-    <mergeCell ref="AF44:AH44"/>
-    <mergeCell ref="AF45:AH45"/>
-    <mergeCell ref="AF36:AH36"/>
-    <mergeCell ref="AF37:AH37"/>
-    <mergeCell ref="AF38:AH38"/>
-    <mergeCell ref="AF39:AH39"/>
-    <mergeCell ref="AF40:AH40"/>
-    <mergeCell ref="AF31:AH31"/>
-    <mergeCell ref="AF32:AH32"/>
-    <mergeCell ref="AF33:AH33"/>
-    <mergeCell ref="AF34:AH34"/>
-    <mergeCell ref="AF35:AH35"/>
-    <mergeCell ref="AF23:AH23"/>
-    <mergeCell ref="AF24:AH24"/>
-    <mergeCell ref="AF25:AH25"/>
-    <mergeCell ref="AF26:AH26"/>
-    <mergeCell ref="AF27:AH27"/>
-    <mergeCell ref="AN56:AP56"/>
-    <mergeCell ref="AN57:AP57"/>
-    <mergeCell ref="AN58:AP58"/>
-    <mergeCell ref="AN59:AP59"/>
-    <mergeCell ref="AN60:AP60"/>
-    <mergeCell ref="AN51:AP51"/>
-    <mergeCell ref="AN52:AP52"/>
-    <mergeCell ref="AN53:AP53"/>
-    <mergeCell ref="AN54:AP54"/>
-    <mergeCell ref="AN55:AP55"/>
-    <mergeCell ref="AN46:AP46"/>
-    <mergeCell ref="AN47:AP47"/>
-    <mergeCell ref="AN48:AP48"/>
-    <mergeCell ref="AN49:AP49"/>
-    <mergeCell ref="AN50:AP50"/>
-    <mergeCell ref="AN41:AP41"/>
-    <mergeCell ref="AN42:AP42"/>
-    <mergeCell ref="AN43:AP43"/>
-    <mergeCell ref="AN44:AP44"/>
-    <mergeCell ref="AN45:AP45"/>
-    <mergeCell ref="AN36:AP36"/>
-    <mergeCell ref="AN37:AP37"/>
-    <mergeCell ref="AN38:AP38"/>
-    <mergeCell ref="AN39:AP39"/>
-    <mergeCell ref="AN40:AP40"/>
-    <mergeCell ref="AN31:AP31"/>
-    <mergeCell ref="AN32:AP32"/>
-    <mergeCell ref="AN33:AP33"/>
-    <mergeCell ref="AN34:AP34"/>
-    <mergeCell ref="AN35:AP35"/>
+  <mergeCells count="143">
     <mergeCell ref="U80:AA80"/>
     <mergeCell ref="AM6:AS6"/>
     <mergeCell ref="AR26:AU26"/>
@@ -6408,7 +6409,40 @@
     <mergeCell ref="AF28:AH28"/>
     <mergeCell ref="AF29:AH29"/>
     <mergeCell ref="AF30:AH30"/>
-    <mergeCell ref="AM2:AP2"/>
+    <mergeCell ref="AR32:AU32"/>
+    <mergeCell ref="AR33:AU33"/>
+    <mergeCell ref="AR34:AU34"/>
+    <mergeCell ref="AR35:AU35"/>
+    <mergeCell ref="AR36:AU36"/>
+    <mergeCell ref="AF49:AH49"/>
+    <mergeCell ref="AF50:AH50"/>
+    <mergeCell ref="AR25:AU25"/>
+    <mergeCell ref="AR47:AU47"/>
+    <mergeCell ref="AR48:AU48"/>
+    <mergeCell ref="AR31:AU31"/>
+    <mergeCell ref="AR56:AU56"/>
+    <mergeCell ref="AR57:AU57"/>
+    <mergeCell ref="AR39:AU39"/>
+    <mergeCell ref="AF38:AH38"/>
+    <mergeCell ref="AF39:AH39"/>
+    <mergeCell ref="AF41:AH41"/>
+    <mergeCell ref="AF42:AH42"/>
+    <mergeCell ref="AF43:AH43"/>
+    <mergeCell ref="AF44:AH44"/>
+    <mergeCell ref="AF45:AH45"/>
+    <mergeCell ref="AF40:AH40"/>
+    <mergeCell ref="AF31:AH31"/>
+    <mergeCell ref="AF32:AH32"/>
+    <mergeCell ref="AF33:AH33"/>
+    <mergeCell ref="AF34:AH34"/>
+    <mergeCell ref="AF35:AH35"/>
+    <mergeCell ref="AF46:AH46"/>
+    <mergeCell ref="AF47:AH47"/>
+    <mergeCell ref="AF48:AH48"/>
+    <mergeCell ref="AN31:AP31"/>
+    <mergeCell ref="AF52:AH52"/>
+    <mergeCell ref="AR37:AU37"/>
+    <mergeCell ref="AR38:AU38"/>
     <mergeCell ref="AR59:AU59"/>
     <mergeCell ref="AR60:AU60"/>
     <mergeCell ref="AR62:AU62"/>
@@ -6423,22 +6457,21 @@
     <mergeCell ref="AR52:AU52"/>
     <mergeCell ref="AR53:AU53"/>
     <mergeCell ref="AR54:AU54"/>
-    <mergeCell ref="AR25:AU25"/>
-    <mergeCell ref="AR47:AU47"/>
-    <mergeCell ref="AR48:AU48"/>
-    <mergeCell ref="AR31:AU31"/>
-    <mergeCell ref="AR56:AU56"/>
-    <mergeCell ref="AR57:AU57"/>
-    <mergeCell ref="AR39:AU39"/>
-    <mergeCell ref="AR40:AU40"/>
+    <mergeCell ref="AF37:AH37"/>
+    <mergeCell ref="AF53:AH53"/>
+    <mergeCell ref="AF54:AH54"/>
+    <mergeCell ref="AF55:AH55"/>
+    <mergeCell ref="AF56:AH56"/>
+    <mergeCell ref="AF57:AH57"/>
+    <mergeCell ref="AN60:AP60"/>
+    <mergeCell ref="AN53:AP53"/>
+    <mergeCell ref="AN54:AP54"/>
+    <mergeCell ref="AN55:AP55"/>
+    <mergeCell ref="AN56:AP56"/>
+    <mergeCell ref="AN57:AP57"/>
+    <mergeCell ref="AN58:AP58"/>
+    <mergeCell ref="AN59:AP59"/>
     <mergeCell ref="AR55:AU55"/>
-    <mergeCell ref="AR32:AU32"/>
-    <mergeCell ref="AR33:AU33"/>
-    <mergeCell ref="AR34:AU34"/>
-    <mergeCell ref="AR35:AU35"/>
-    <mergeCell ref="AR36:AU36"/>
-    <mergeCell ref="AR37:AU37"/>
-    <mergeCell ref="AR38:AU38"/>
     <mergeCell ref="AJ89:AS89"/>
     <mergeCell ref="AR67:AU67"/>
     <mergeCell ref="AR58:AU58"/>
@@ -6447,13 +6480,6 @@
     <mergeCell ref="AF59:AH59"/>
     <mergeCell ref="AF60:AH60"/>
     <mergeCell ref="AF61:AH61"/>
-    <mergeCell ref="AF53:AH53"/>
-    <mergeCell ref="AF54:AH54"/>
-    <mergeCell ref="AF55:AH55"/>
-    <mergeCell ref="AF56:AH56"/>
-    <mergeCell ref="AF57:AH57"/>
-    <mergeCell ref="AF51:AH51"/>
-    <mergeCell ref="AF52:AH52"/>
     <mergeCell ref="Y69:Z69"/>
     <mergeCell ref="AR23:AU23"/>
     <mergeCell ref="AR24:AU24"/>
@@ -6470,6 +6496,35 @@
     <mergeCell ref="AF19:AH19"/>
     <mergeCell ref="AF20:AH20"/>
     <mergeCell ref="AF21:AH21"/>
+    <mergeCell ref="AN51:AP51"/>
+    <mergeCell ref="AN52:AP52"/>
+    <mergeCell ref="AN46:AP46"/>
+    <mergeCell ref="AN47:AP47"/>
+    <mergeCell ref="AN48:AP48"/>
+    <mergeCell ref="AN49:AP49"/>
+    <mergeCell ref="AN50:AP50"/>
+    <mergeCell ref="AR40:AU40"/>
+    <mergeCell ref="AF51:AH51"/>
+    <mergeCell ref="AF23:AH23"/>
+    <mergeCell ref="AF24:AH24"/>
+    <mergeCell ref="AF25:AH25"/>
+    <mergeCell ref="AF26:AH26"/>
+    <mergeCell ref="AF27:AH27"/>
+    <mergeCell ref="AN41:AP41"/>
+    <mergeCell ref="AN42:AP42"/>
+    <mergeCell ref="AN43:AP43"/>
+    <mergeCell ref="AN44:AP44"/>
+    <mergeCell ref="AN45:AP45"/>
+    <mergeCell ref="AN36:AP36"/>
+    <mergeCell ref="AN37:AP37"/>
+    <mergeCell ref="AN38:AP38"/>
+    <mergeCell ref="AN39:AP39"/>
+    <mergeCell ref="AN40:AP40"/>
+    <mergeCell ref="AN32:AP32"/>
+    <mergeCell ref="AN33:AP33"/>
+    <mergeCell ref="AN34:AP34"/>
+    <mergeCell ref="AN35:AP35"/>
+    <mergeCell ref="AF36:AH36"/>
     <mergeCell ref="F12:K12"/>
     <mergeCell ref="Y10:AE10"/>
     <mergeCell ref="AR22:AU22"/>
@@ -6478,6 +6533,8 @@
     <mergeCell ref="AR21:AU21"/>
     <mergeCell ref="AI10:AK10"/>
     <mergeCell ref="AF22:AH22"/>
+    <mergeCell ref="AM2:AN2"/>
+    <mergeCell ref="AM8:AN8"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.51181102362204722" top="0.55118110236220474" bottom="0.55118110236220474" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="65" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
@@ -6486,7 +6543,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -6522,60 +6579,60 @@
       <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B3" s="139" t="s">
+      <c r="B3" s="165" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="139"/>
+      <c r="C3" s="165"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="139" t="s">
+      <c r="B4" s="165" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="139"/>
+      <c r="C4" s="165"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="139" t="s">
+      <c r="B5" s="165" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="139"/>
+      <c r="C5" s="165"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="139" t="s">
+      <c r="B6" s="165" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="139"/>
+      <c r="C6" s="165"/>
     </row>
     <row r="7" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="143" t="s">
+      <c r="B7" s="169" t="s">
         <v>96</v>
       </c>
-      <c r="C7" s="143"/>
-      <c r="D7" s="143"/>
+      <c r="C7" s="169"/>
+      <c r="D7" s="169"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="139" t="s">
+      <c r="B8" s="165" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="139"/>
+      <c r="C8" s="165"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="141" t="s">
+      <c r="B9" s="167" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="141"/>
+      <c r="C9" s="167"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="139" t="s">
+      <c r="B10" s="165" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="139"/>
+      <c r="C10" s="165"/>
     </row>
     <row r="11" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="143" t="s">
+      <c r="B11" s="169" t="s">
         <v>95</v>
       </c>
-      <c r="C11" s="143"/>
-      <c r="D11" s="143"/>
+      <c r="C11" s="169"/>
+      <c r="D11" s="169"/>
     </row>
     <row r="12" spans="1:5" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
@@ -6587,40 +6644,40 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="142" t="s">
+      <c r="B13" s="168" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="141"/>
+      <c r="C13" s="167"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B14" s="139" t="s">
+      <c r="B14" s="165" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="139"/>
+      <c r="C14" s="165"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="139" t="s">
+      <c r="B15" s="165" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="139"/>
+      <c r="C15" s="165"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B16" s="139" t="s">
+      <c r="B16" s="165" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="139"/>
+      <c r="C16" s="165"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B17" s="139" t="s">
+      <c r="B17" s="165" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="139"/>
+      <c r="C17" s="165"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B18" s="139" t="s">
+      <c r="B18" s="165" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="139"/>
+      <c r="C18" s="165"/>
     </row>
     <row r="19" spans="1:5" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
@@ -6632,100 +6689,100 @@
       <c r="E19" s="5"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B20" s="139" t="s">
+      <c r="B20" s="165" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="139"/>
+      <c r="C20" s="165"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B21" s="139" t="s">
+      <c r="B21" s="165" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="139"/>
+      <c r="C21" s="165"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B22" s="139" t="s">
+      <c r="B22" s="165" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="139"/>
+      <c r="C22" s="165"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B23" s="139" t="s">
+      <c r="B23" s="165" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="139"/>
+      <c r="C23" s="165"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B24" s="139" t="s">
+      <c r="B24" s="165" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="139"/>
+      <c r="C24" s="165"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B25" s="139" t="s">
+      <c r="B25" s="165" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="139"/>
+      <c r="C25" s="165"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B26" s="139" t="s">
+      <c r="B26" s="165" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="139"/>
+      <c r="C26" s="165"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B27" s="139" t="s">
+      <c r="B27" s="165" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="139"/>
+      <c r="C27" s="165"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B28" s="139" t="s">
+      <c r="B28" s="165" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="139"/>
+      <c r="C28" s="165"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B29" s="139" t="s">
+      <c r="B29" s="165" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="139"/>
+      <c r="C29" s="165"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B30" s="139" t="s">
+      <c r="B30" s="165" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="139"/>
+      <c r="C30" s="165"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B31" s="139" t="s">
+      <c r="B31" s="165" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="139"/>
+      <c r="C31" s="165"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B32" s="139" t="s">
+      <c r="B32" s="165" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="139"/>
+      <c r="C32" s="165"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B33" s="139" t="s">
+      <c r="B33" s="165" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="139"/>
+      <c r="C33" s="165"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B34" s="139" t="s">
+      <c r="B34" s="165" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="139"/>
+      <c r="C34" s="165"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B35" s="139" t="s">
+      <c r="B35" s="165" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="139"/>
+      <c r="C35" s="165"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B36" s="21" t="s">
@@ -6733,28 +6790,28 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B37" s="139" t="s">
+      <c r="B37" s="165" t="s">
         <v>37</v>
       </c>
-      <c r="C37" s="139"/>
+      <c r="C37" s="165"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B38" s="139" t="s">
+      <c r="B38" s="165" t="s">
         <v>38</v>
       </c>
-      <c r="C38" s="139"/>
+      <c r="C38" s="165"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B39" s="139" t="s">
+      <c r="B39" s="165" t="s">
         <v>39</v>
       </c>
-      <c r="C39" s="139"/>
+      <c r="C39" s="165"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B40" s="139" t="s">
+      <c r="B40" s="165" t="s">
         <v>40</v>
       </c>
-      <c r="C40" s="139"/>
+      <c r="C40" s="165"/>
     </row>
     <row r="41" spans="1:5" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
@@ -6766,35 +6823,35 @@
       <c r="E41" s="5"/>
     </row>
     <row r="42" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="143" t="s">
+      <c r="B42" s="169" t="s">
         <v>97</v>
       </c>
-      <c r="C42" s="143"/>
-      <c r="D42" s="143"/>
+      <c r="C42" s="169"/>
+      <c r="D42" s="169"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B43" s="139" t="s">
+      <c r="B43" s="165" t="s">
         <v>42</v>
       </c>
-      <c r="C43" s="139"/>
+      <c r="C43" s="165"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B44" s="139" t="s">
+      <c r="B44" s="165" t="s">
         <v>43</v>
       </c>
-      <c r="C44" s="139"/>
+      <c r="C44" s="165"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B45" s="139" t="s">
+      <c r="B45" s="165" t="s">
         <v>44</v>
       </c>
-      <c r="C45" s="139"/>
+      <c r="C45" s="165"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B46" s="139" t="s">
+      <c r="B46" s="165" t="s">
         <v>45</v>
       </c>
-      <c r="C46" s="139"/>
+      <c r="C46" s="165"/>
     </row>
     <row r="47" spans="1:5" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
@@ -6806,40 +6863,40 @@
       <c r="E47" s="5"/>
     </row>
     <row r="48" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B48" s="141" t="s">
+      <c r="B48" s="167" t="s">
         <v>53</v>
       </c>
-      <c r="C48" s="141"/>
+      <c r="C48" s="167"/>
     </row>
     <row r="49" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="139" t="s">
+      <c r="B49" s="165" t="s">
         <v>47</v>
       </c>
-      <c r="C49" s="139"/>
+      <c r="C49" s="165"/>
     </row>
     <row r="50" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="139" t="s">
+      <c r="B50" s="165" t="s">
         <v>54</v>
       </c>
-      <c r="C50" s="139"/>
+      <c r="C50" s="165"/>
     </row>
     <row r="51" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B51" s="139" t="s">
+      <c r="B51" s="165" t="s">
         <v>48</v>
       </c>
-      <c r="C51" s="139"/>
+      <c r="C51" s="165"/>
     </row>
     <row r="52" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B52" s="139" t="s">
+      <c r="B52" s="165" t="s">
         <v>49</v>
       </c>
-      <c r="C52" s="139"/>
+      <c r="C52" s="165"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B53" s="139" t="s">
+      <c r="B53" s="165" t="s">
         <v>50</v>
       </c>
-      <c r="C53" s="139"/>
+      <c r="C53" s="165"/>
     </row>
     <row r="54" spans="1:6" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
@@ -6851,11 +6908,11 @@
       <c r="E54" s="5"/>
     </row>
     <row r="55" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B55" s="144" t="s">
+      <c r="B55" s="170" t="s">
         <v>55</v>
       </c>
-      <c r="C55" s="144"/>
-      <c r="D55" s="144"/>
+      <c r="C55" s="170"/>
+      <c r="D55" s="170"/>
       <c r="F55" s="6"/>
     </row>
     <row r="56" spans="1:6" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -6868,52 +6925,52 @@
       <c r="E56" s="5"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B57" s="142" t="s">
+      <c r="B57" s="168" t="s">
         <v>57</v>
       </c>
-      <c r="C57" s="142"/>
+      <c r="C57" s="168"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B58" s="140" t="s">
+      <c r="B58" s="166" t="s">
         <v>58</v>
       </c>
-      <c r="C58" s="140"/>
+      <c r="C58" s="166"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B59" s="140" t="s">
+      <c r="B59" s="166" t="s">
         <v>59</v>
       </c>
-      <c r="C59" s="140"/>
+      <c r="C59" s="166"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B60" s="140" t="s">
+      <c r="B60" s="166" t="s">
         <v>60</v>
       </c>
-      <c r="C60" s="140"/>
+      <c r="C60" s="166"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B61" s="140" t="s">
+      <c r="B61" s="166" t="s">
         <v>61</v>
       </c>
-      <c r="C61" s="140"/>
+      <c r="C61" s="166"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B62" s="140" t="s">
+      <c r="B62" s="166" t="s">
         <v>62</v>
       </c>
-      <c r="C62" s="140"/>
+      <c r="C62" s="166"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B63" s="140" t="s">
+      <c r="B63" s="166" t="s">
         <v>63</v>
       </c>
-      <c r="C63" s="140"/>
+      <c r="C63" s="166"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B64" s="140" t="s">
+      <c r="B64" s="166" t="s">
         <v>65</v>
       </c>
-      <c r="C64" s="140"/>
+      <c r="C64" s="166"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
@@ -6921,25 +6978,25 @@
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B66" s="140" t="s">
+      <c r="B66" s="166" t="s">
         <v>72</v>
       </c>
-      <c r="C66" s="140"/>
+      <c r="C66" s="166"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B67" s="140" t="s">
+      <c r="B67" s="166" t="s">
         <v>73</v>
       </c>
-      <c r="C67" s="140"/>
+      <c r="C67" s="166"/>
     </row>
     <row r="69" spans="1:5" ht="123" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B69" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="C69" s="137" t="s">
+      <c r="C69" s="163" t="s">
         <v>111</v>
       </c>
-      <c r="D69" s="138"/>
+      <c r="D69" s="164"/>
       <c r="E69" s="7"/>
     </row>
   </sheetData>

</xml_diff>